<commit_message>
fixed intendention of second tree
</commit_message>
<xml_diff>
--- a/02_work_doc/01_daten/08_criteriaCatalog/Tabelle_Wissensplattform_criteriaCatalog_Personalisierung.xlsx
+++ b/02_work_doc/01_daten/08_criteriaCatalog/Tabelle_Wissensplattform_criteriaCatalog_Personalisierung.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="99">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -37,6 +37,9 @@
     <t xml:space="preserve">parentId</t>
   </si>
   <si>
+    <t xml:space="preserve">image</t>
+  </si>
+  <si>
     <t xml:space="preserve">Profilbildung und Personalisierung</t>
   </si>
   <si>
@@ -44,6 +47,9 @@
   </si>
   <si>
     <t xml:space="preserve">Kurz &amp; bündig: Es wird spezifiziert, ob und welche personenbezogenen Daten verarbeitet werden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data.svg</t>
   </si>
   <si>
     <t xml:space="preserve">Spezifikation der Datenkategorien</t>
@@ -345,6 +351,9 @@
     <t xml:space="preserve">Die Zwecke der Datenverarbeitung werden richtig spezifiziert</t>
   </si>
   <si>
+    <t xml:space="preserve">flag.svg</t>
+  </si>
+  <si>
     <t xml:space="preserve">Korrekte Spezifizierung des Verarbeitungszwecks</t>
   </si>
   <si>
@@ -421,7 +430,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -450,6 +459,12 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
       <b val="true"/>
@@ -515,7 +530,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -528,11 +543,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -540,7 +559,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -683,10 +702,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D60" activeCellId="0" sqref="D60"/>
+      <selection pane="bottomLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.62"/>
@@ -694,7 +713,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.62"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -710,7 +729,9 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2"/>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -732,21 +753,23 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="F2" s="3" t="s">
+        <v>9</v>
+      </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -768,18 +791,18 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2" t="n">
         <f aca="false">A2</f>
@@ -812,10 +835,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="n">
@@ -849,13 +872,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E5" s="2" t="n">
         <f aca="false">A4</f>
@@ -888,13 +911,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E6" s="2" t="n">
         <f aca="false">A4</f>
@@ -927,13 +950,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E7" s="2" t="n">
         <f aca="false">A4</f>
@@ -966,10 +989,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="n">
@@ -1003,13 +1026,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>19</v>
+      <c r="D9" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="E9" s="2" t="n">
         <f aca="false">A8</f>
@@ -1042,13 +1065,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>20</v>
+      <c r="C10" s="5" t="s">
+        <v>22</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>21</v>
+      <c r="D10" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="E10" s="2" t="n">
         <f aca="false">A8</f>
@@ -1080,13 +1103,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>22</v>
+      <c r="C11" s="5" t="s">
+        <v>24</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>23</v>
+      <c r="D11" s="6" t="s">
+        <v>25</v>
       </c>
       <c r="E11" s="2" t="n">
         <f aca="false">A8</f>
@@ -1118,13 +1141,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>25</v>
+      <c r="D12" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="E12" s="2" t="n">
         <f aca="false">A2</f>
@@ -1152,15 +1175,15 @@
       <c r="Y12" s="2"/>
       <c r="Z12" s="2"/>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="n">
@@ -1189,15 +1212,15 @@
       <c r="Y13" s="2"/>
       <c r="Z13" s="2"/>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="n">
@@ -1226,15 +1249,15 @@
       <c r="Y14" s="2"/>
       <c r="Z14" s="2"/>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2" t="n">
@@ -1263,18 +1286,18 @@
       <c r="Y15" s="2"/>
       <c r="Z15" s="2"/>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
-      <c r="D16" s="6" t="s">
-        <v>30</v>
+      <c r="D16" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="E16" s="2" t="n">
         <f aca="false">A15</f>
@@ -1302,18 +1325,18 @@
       <c r="Y16" s="2"/>
       <c r="Z16" s="2"/>
     </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="n">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>31</v>
+      <c r="C17" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E17" s="2" t="n">
         <f aca="false">A15</f>
@@ -1341,15 +1364,15 @@
       <c r="Y17" s="2"/>
       <c r="Z17" s="2"/>
     </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2" t="n">
@@ -1378,18 +1401,18 @@
       <c r="Y18" s="2"/>
       <c r="Z18" s="2"/>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E19" s="2" t="n">
         <f aca="false">A18</f>
@@ -1417,18 +1440,18 @@
       <c r="Y19" s="2"/>
       <c r="Z19" s="2"/>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="n">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E20" s="2" t="n">
         <f aca="false">A14</f>
@@ -1456,15 +1479,15 @@
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="n">
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2" t="n">
@@ -1493,15 +1516,15 @@
       <c r="Y21" s="2"/>
       <c r="Z21" s="2"/>
     </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="n">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2" t="n">
@@ -1530,18 +1553,18 @@
       <c r="Y22" s="2"/>
       <c r="Z22" s="2"/>
     </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="n">
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E23" s="2" t="n">
         <f aca="false">A22</f>
@@ -1569,18 +1592,18 @@
       <c r="Y23" s="2"/>
       <c r="Z23" s="2"/>
     </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="n">
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>41</v>
+      <c r="C24" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E24" s="2" t="n">
         <f aca="false">A22</f>
@@ -1608,18 +1631,18 @@
       <c r="Y24" s="2"/>
       <c r="Z24" s="2"/>
     </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="n">
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E25" s="2" t="n">
         <f aca="false">A21</f>
@@ -1652,13 +1675,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>46</v>
+      <c r="D26" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="E26" s="2" t="n">
         <f aca="false">A2</f>
@@ -1686,15 +1709,15 @@
       <c r="Y26" s="2"/>
       <c r="Z26" s="2"/>
     </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="n">
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2" t="n">
@@ -1728,13 +1751,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>49</v>
+      <c r="D28" s="4" t="s">
+        <v>51</v>
       </c>
       <c r="E28" s="2" t="n">
         <f aca="false">A27</f>
@@ -1767,13 +1790,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>51</v>
+      <c r="D29" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="E29" s="2" t="n">
         <f aca="false">A27</f>
@@ -1806,13 +1829,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>53</v>
+      <c r="D30" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="E30" s="2" t="n">
         <f aca="false">A27</f>
@@ -1840,18 +1863,18 @@
       <c r="Y30" s="2"/>
       <c r="Z30" s="2"/>
     </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="n">
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E31" s="2" t="n">
         <f aca="false">A2</f>
@@ -1879,18 +1902,18 @@
       <c r="Y31" s="2"/>
       <c r="Z31" s="2"/>
     </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="n">
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E32" s="2" t="n">
         <f aca="false">A31</f>
@@ -1923,13 +1946,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
-      <c r="D33" s="3" t="s">
-        <v>59</v>
+      <c r="D33" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="E33" s="2" t="n">
         <f aca="false">A32</f>
@@ -1962,13 +1985,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>61</v>
+      <c r="D34" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="E34" s="2" t="n">
         <f aca="false">A32</f>
@@ -2001,13 +2024,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>63</v>
+      <c r="D35" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="E35" s="2" t="n">
         <f aca="false">A32</f>
@@ -2035,18 +2058,18 @@
       <c r="Y35" s="2"/>
       <c r="Z35" s="2"/>
     </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="n">
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E36" s="2" t="n">
         <f aca="false">A31</f>
@@ -2074,18 +2097,18 @@
       <c r="Y36" s="2"/>
       <c r="Z36" s="2"/>
     </row>
-    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="n">
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E37" s="2" t="n">
         <f aca="false">A36</f>
@@ -2118,13 +2141,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
-      <c r="D38" s="3" t="s">
-        <v>69</v>
+      <c r="D38" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="E38" s="2" t="n">
         <f aca="false">A37</f>
@@ -2152,15 +2175,15 @@
       <c r="Y38" s="2"/>
       <c r="Z38" s="2"/>
     </row>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="n">
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2" t="n">
@@ -2189,18 +2212,18 @@
       <c r="Y39" s="2"/>
       <c r="Z39" s="2"/>
     </row>
-    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="n">
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E40" s="2" t="n">
         <f aca="false">A39</f>
@@ -2228,18 +2251,18 @@
       <c r="Y40" s="2"/>
       <c r="Z40" s="2"/>
     </row>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="n">
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E41" s="2" t="n">
         <f aca="false">A39</f>
@@ -2272,13 +2295,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
-      <c r="D42" s="3" t="s">
-        <v>75</v>
+      <c r="D42" s="4" t="s">
+        <v>77</v>
       </c>
       <c r="E42" s="2" t="n">
         <f aca="false">A39</f>
@@ -2311,13 +2334,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>77</v>
+      <c r="D43" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="E43" s="2" t="n">
         <f aca="false">A39</f>
@@ -2345,21 +2368,23 @@
       <c r="Y43" s="2"/>
       <c r="Z43" s="2"/>
     </row>
-    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="n">
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
+      <c r="F44" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
@@ -2386,13 +2411,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
-      <c r="D45" s="3" t="s">
-        <v>81</v>
+      <c r="D45" s="4" t="s">
+        <v>84</v>
       </c>
       <c r="E45" s="2" t="n">
         <f aca="false">A44</f>
@@ -2420,18 +2445,18 @@
       <c r="Y45" s="2"/>
       <c r="Z45" s="2"/>
     </row>
-    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="n">
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="E46" s="2" t="n">
         <f aca="false">A45</f>
@@ -2464,13 +2489,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>85</v>
+      <c r="D47" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="E47" s="2" t="n">
         <f aca="false">A46</f>
@@ -2503,13 +2528,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
-      <c r="D48" s="3" t="s">
-        <v>87</v>
+      <c r="D48" s="4" t="s">
+        <v>90</v>
       </c>
       <c r="E48" s="2" t="n">
         <f aca="false">A46</f>
@@ -2542,13 +2567,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
-      <c r="D49" s="3" t="s">
-        <v>89</v>
+      <c r="D49" s="4" t="s">
+        <v>92</v>
       </c>
       <c r="E49" s="2" t="n">
         <f aca="false">A46</f>
@@ -2581,13 +2606,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="E50" s="2" t="n">
         <f aca="false">A46</f>
@@ -2620,13 +2645,13 @@
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
-      <c r="D51" s="3" t="s">
-        <v>93</v>
+      <c r="D51" s="4" t="s">
+        <v>96</v>
       </c>
       <c r="E51" s="2" t="n">
         <f aca="false">A46</f>
@@ -2659,13 +2684,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="E52" s="2" t="n">
         <f aca="false">A45</f>

</xml_diff>

<commit_message>
merged the two excel-files from Valentin into one file
</commit_message>
<xml_diff>
--- a/02_work_doc/01_daten/08_criteriaCatalog/Tabelle_Wissensplattform_criteriaCatalog_Personalisierung.xlsx
+++ b/02_work_doc/01_daten/08_criteriaCatalog/Tabelle_Wissensplattform_criteriaCatalog_Personalisierung.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="101">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -422,6 +422,31 @@
   <si>
     <t xml:space="preserve">Im Zeitpunkt der Datenerhebung müssen die konkreten Verarbeitungszwecke bereits spezifiziert worden sein. Wenn einzelne Parameter des konkreten Verarbeitungszwecks dem Verantwortlichen noch nicht bekannt sind, kann auch eine spätere Präzisierung des Zwecks zulässig sein, ohne dass hierfür eine neue Rechtsgrundlage und eine neue Datenerhebung erforderlich ist. Dieser Fall der Zweckpräzisierung wird im Rahmen der Zweckbindung dargelegt (siehe Zweckbindung).</t>
   </si>
+  <si>
+    <t xml:space="preserve">Betrieb und Betriebsoptimierung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Energieverbrauchsdaten sind in jedem Fall dem Kernbereich des Privatlebens zuzuordnen, insoweit sich hieraus Informationen über den abgeschirmten Lebensbereich betroffener Personnen innerhalb ihres geschützten Wohnraumes ableiten lassen (häuslicher Bereich als abgeschirmter Kernbereich der Privatssphäre - vgl. BGH,GRUR 1996, 923, 925, siehe auch DSK Stellungnahme zu Funkwasserzählern, 2023).
+- Laut Greveler et al. (2012) lassen sich aus den 
+Daten intelligenter Verbrauchszähler Aussagen darüber treffen, welche Fernsehprogramme angeschaut werden 
+- Es sind aber "räumliche, zeitliche und soziale Kontextinformationen notwendig [...], um detailreiche und kontextabhängige Informationen zu erhalten" vgl. Richter et al. (2018), S. 131 --&gt; z.B. bzgl. der Identifizierung einzelner elektronischer Geräte aus Smart-Meter Daten: 
+werden: Leistungsaufnahme, Funktionsweise/Lastprofil einzelner Gerätetypen, typische Arbeitszyklen, Nutzungszeitpunkte, Verwendungshäufigkeit (Müller, DuD 2010, 359, 361)
+Wohngebäude:
+Alle von einem Smart Meter erhobenen Energieverbrauchsdaten sind personenbezogene Daten, insoweit sie sich auf eine Wohneinheit zurückführen lassen.
+Ableitbare Informationen:
+- aus Lastprofilen (idR 15-minütige Abtastung)  lässt sich erkennen, welche Geräte im Haushalt wann benutzt werden - vgl. Nyquist-Shannon-Abtasttheorem, wonach nur Schaltvorgänge erkennbar sind, die maximal die halbe Periodendauer der Abtastung haben (vgl. am Beispiel des Kühlschranks in: Müller, DuD 2010, 359, 362, dessen Lastprofil ab einer 15-minütigen Messfrequenz erkennbar wird).
+- daraus lassen sich weitere Informationen über das Verhalten von Personen, insb. Gewohnheiten des täglichen Lebens ableiten:
+Zu welcher Uhrzeit geht der Nutzer zu Bett? Zu welcher Uhrzeit steht er auf? Gibt es nächtliche Toilettenbesuche? Wie häufig kocht er? Benutzt er regelmäßig den Backofen? Wann verlässt er das Haus? Wann kommt er zurück? Wie häufig wird das Baby gewickelt (Heizstrahler über dem Wickeltisch) Verändern sich die Lebensgewohnheiten (Nachwuchs, Besuch)? (Müller, DuD 2010, 359, 361)
+Identifizierbarkeit (konk. Risiko für Privatleben):
+- Informationen lassen sich über Vertrag zw. Energielieferant und Vertragsnehmer auf diesen zurückführen (vgl. BfDI, Orientierungshilfe datenschutzgerechtes Smart Metering, S. 8; Keppeler, EnWZ 2016, 99, 100)
+- hinsichtlich anderer Mitbewohner? z.B. über IP-Adressen der Hausmitbewohner (zum Für und Wider: Keppeler, EnWZ 2016, 99, 101)
+- im Übrigen: Telefonbuch, Klingelschild etc.
+Technisch-Organisatorische Maßnahmen:
+- geringere zeitl. Auflösung
+- Aggregation der Zwischenwerte
+- Aggregation mehrerer Haushalte
+detailiert hierzu (Müller, DuD 2010, 359, 362)</t>
+  </si>
 </sst>
 </file>
 
@@ -430,7 +455,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -461,12 +486,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -476,6 +495,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="&quot;Arial&quot;"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="&quot;Arial&quot;"/>
       <family val="0"/>
@@ -530,7 +564,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -543,15 +577,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -559,7 +589,27 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -702,10 +752,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
+      <selection pane="bottomLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.62"/>
@@ -767,7 +817,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="2"/>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G2" s="2"/>
@@ -1031,7 +1081,7 @@
       <c r="C9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E9" s="2" t="n">
@@ -1067,10 +1117,10 @@
       <c r="B10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E10" s="2" t="n">
@@ -1105,10 +1155,10 @@
       <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>25</v>
       </c>
       <c r="E11" s="2" t="n">
@@ -1146,7 +1196,7 @@
       <c r="C12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E12" s="2" t="n">
@@ -1296,7 +1346,7 @@
       <c r="C16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="6" t="s">
         <v>32</v>
       </c>
       <c r="E16" s="2" t="n">
@@ -1332,7 +1382,7 @@
       <c r="B17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>33</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -1599,7 +1649,7 @@
       <c r="B24" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="6" t="s">
         <v>43</v>
       </c>
       <c r="D24" s="2" t="s">
@@ -1680,7 +1730,7 @@
       <c r="C26" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="3" t="s">
         <v>48</v>
       </c>
       <c r="E26" s="2" t="n">
@@ -1756,7 +1806,7 @@
       <c r="C28" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E28" s="2" t="n">
@@ -1795,7 +1845,7 @@
       <c r="C29" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="3" t="s">
         <v>53</v>
       </c>
       <c r="E29" s="2" t="n">
@@ -1834,7 +1884,7 @@
       <c r="C30" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="D30" s="3" t="s">
         <v>55</v>
       </c>
       <c r="E30" s="2" t="n">
@@ -1951,7 +2001,7 @@
       <c r="C33" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D33" s="4" t="s">
+      <c r="D33" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E33" s="2" t="n">
@@ -1990,7 +2040,7 @@
       <c r="C34" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="D34" s="3" t="s">
         <v>63</v>
       </c>
       <c r="E34" s="2" t="n">
@@ -2029,7 +2079,7 @@
       <c r="C35" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D35" s="4" t="s">
+      <c r="D35" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E35" s="2" t="n">
@@ -2146,7 +2196,7 @@
       <c r="C38" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" s="3" t="s">
         <v>71</v>
       </c>
       <c r="E38" s="2" t="n">
@@ -2300,7 +2350,7 @@
       <c r="C42" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="D42" s="3" t="s">
         <v>77</v>
       </c>
       <c r="E42" s="2" t="n">
@@ -2339,7 +2389,7 @@
       <c r="C43" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="D43" s="3" t="s">
         <v>79</v>
       </c>
       <c r="E43" s="2" t="n">
@@ -2416,7 +2466,7 @@
       <c r="C45" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="D45" s="3" t="s">
         <v>84</v>
       </c>
       <c r="E45" s="2" t="n">
@@ -2494,7 +2544,7 @@
       <c r="C47" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D47" s="4" t="s">
+      <c r="D47" s="3" t="s">
         <v>88</v>
       </c>
       <c r="E47" s="2" t="n">
@@ -2533,7 +2583,7 @@
       <c r="C48" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D48" s="4" t="s">
+      <c r="D48" s="3" t="s">
         <v>90</v>
       </c>
       <c r="E48" s="2" t="n">
@@ -2572,7 +2622,7 @@
       <c r="C49" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D49" s="4" t="s">
+      <c r="D49" s="3" t="s">
         <v>92</v>
       </c>
       <c r="E49" s="2" t="n">
@@ -2650,7 +2700,7 @@
       <c r="C51" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="D51" s="3" t="s">
         <v>96</v>
       </c>
       <c r="E51" s="2" t="n">
@@ -2719,13 +2769,22 @@
       <c r="Z52" s="2"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="2"/>
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
-      <c r="G53" s="2"/>
+      <c r="A53" s="7" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" s="7"/>
+      <c r="F53" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
@@ -2747,13 +2806,23 @@
       <c r="Z53" s="2"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="2"/>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
+      <c r="A54" s="7" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54" s="7" t="n">
+        <f aca="false">A53</f>
+        <v>52</v>
+      </c>
       <c r="F54" s="2"/>
-      <c r="G54" s="2"/>
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
@@ -2775,12 +2844,21 @@
       <c r="Z54" s="2"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
+      <c r="A55" s="7" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7" t="n">
+        <f aca="false">A54</f>
+        <v>53</v>
+      </c>
       <c r="F55" s="2"/>
-      <c r="G55" s="2"/>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
@@ -2802,12 +2880,23 @@
       <c r="Z55" s="2"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
+      <c r="A56" s="7" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E56" s="7" t="n">
+        <f aca="false">A55</f>
+        <v>54</v>
+      </c>
       <c r="F56" s="2"/>
-      <c r="G56" s="2"/>
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
@@ -2829,12 +2918,23 @@
       <c r="Z56" s="2"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2"/>
+      <c r="A57" s="7" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E57" s="7" t="n">
+        <f aca="false">A55</f>
+        <v>54</v>
+      </c>
       <c r="F57" s="2"/>
-      <c r="G57" s="2"/>
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
@@ -2856,12 +2956,23 @@
       <c r="Z57" s="2"/>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
-      <c r="E58" s="2"/>
+      <c r="A58" s="7" t="n">
+        <v>57</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E58" s="7" t="n">
+        <f aca="false">A55</f>
+        <v>54</v>
+      </c>
       <c r="F58" s="2"/>
-      <c r="G58" s="2"/>
       <c r="H58" s="2"/>
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
@@ -2883,12 +2994,21 @@
       <c r="Z58" s="2"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
+      <c r="A59" s="7" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D59" s="7"/>
+      <c r="E59" s="7" t="n">
+        <f aca="false">A55</f>
+        <v>54</v>
+      </c>
       <c r="F59" s="2"/>
-      <c r="G59" s="2"/>
       <c r="H59" s="2"/>
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
@@ -2909,13 +3029,24 @@
       <c r="Y59" s="2"/>
       <c r="Z59" s="2"/>
     </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
-      <c r="E60" s="2"/>
+    <row r="60" customFormat="false" ht="173.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="7" t="n">
+        <v>59</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E60" s="7" t="n">
+        <f aca="false">A59</f>
+        <v>58</v>
+      </c>
       <c r="F60" s="2"/>
-      <c r="G60" s="2"/>
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
@@ -2936,13 +3067,24 @@
       <c r="Y60" s="2"/>
       <c r="Z60" s="2"/>
     </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
-      <c r="E61" s="2"/>
+    <row r="61" customFormat="false" ht="276.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="7" t="n">
+        <v>60</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D61" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="E61" s="7" t="n">
+        <f aca="false">A59</f>
+        <v>58</v>
+      </c>
       <c r="F61" s="2"/>
-      <c r="G61" s="2"/>
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
@@ -2963,13 +3105,24 @@
       <c r="Y61" s="2"/>
       <c r="Z61" s="2"/>
     </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
-      <c r="D62" s="2"/>
-      <c r="E62" s="2"/>
+    <row r="62" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="7" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D62" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E62" s="7" t="n">
+        <f aca="false">A59</f>
+        <v>58</v>
+      </c>
       <c r="F62" s="2"/>
-      <c r="G62" s="2"/>
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
@@ -2990,13 +3143,24 @@
       <c r="Y62" s="2"/>
       <c r="Z62" s="2"/>
     </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
-      <c r="D63" s="2"/>
-      <c r="E63" s="2"/>
+    <row r="63" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="7" t="n">
+        <v>62</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E63" s="7" t="n">
+        <f aca="false">A53</f>
+        <v>52</v>
+      </c>
       <c r="F63" s="2"/>
-      <c r="G63" s="2"/>
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
@@ -3018,12 +3182,21 @@
       <c r="Z63" s="2"/>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2"/>
-      <c r="E64" s="2"/>
+      <c r="A64" s="7" t="n">
+        <v>63</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D64" s="7"/>
+      <c r="E64" s="7" t="n">
+        <f aca="false">A63</f>
+        <v>62</v>
+      </c>
       <c r="F64" s="2"/>
-      <c r="G64" s="2"/>
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
@@ -3045,12 +3218,21 @@
       <c r="Z64" s="2"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="2"/>
-      <c r="C65" s="2"/>
-      <c r="D65" s="2"/>
-      <c r="E65" s="2"/>
+      <c r="A65" s="7" t="n">
+        <v>64</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D65" s="7"/>
+      <c r="E65" s="7" t="n">
+        <f aca="false">A64</f>
+        <v>63</v>
+      </c>
       <c r="F65" s="2"/>
-      <c r="G65" s="2"/>
       <c r="H65" s="2"/>
       <c r="I65" s="2"/>
       <c r="J65" s="2"/>
@@ -3072,12 +3254,21 @@
       <c r="Z65" s="2"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B66" s="2"/>
-      <c r="C66" s="2"/>
-      <c r="D66" s="2"/>
-      <c r="E66" s="2"/>
+      <c r="A66" s="7" t="n">
+        <v>65</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D66" s="7"/>
+      <c r="E66" s="7" t="n">
+        <f aca="false">A65</f>
+        <v>64</v>
+      </c>
       <c r="F66" s="2"/>
-      <c r="G66" s="2"/>
       <c r="H66" s="2"/>
       <c r="I66" s="2"/>
       <c r="J66" s="2"/>
@@ -3099,12 +3290,23 @@
       <c r="Z66" s="2"/>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
-      <c r="D67" s="2"/>
-      <c r="E67" s="2"/>
+      <c r="A67" s="7" t="n">
+        <v>66</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D67" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E67" s="7" t="n">
+        <f aca="false">A66</f>
+        <v>65</v>
+      </c>
       <c r="F67" s="2"/>
-      <c r="G67" s="2"/>
       <c r="H67" s="2"/>
       <c r="I67" s="2"/>
       <c r="J67" s="2"/>
@@ -3126,12 +3328,23 @@
       <c r="Z67" s="2"/>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="2"/>
-      <c r="C68" s="2"/>
-      <c r="D68" s="2"/>
-      <c r="E68" s="2"/>
+      <c r="A68" s="7" t="n">
+        <v>67</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C68" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D68" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E68" s="7" t="n">
+        <f aca="false">A66</f>
+        <v>65</v>
+      </c>
       <c r="F68" s="2"/>
-      <c r="G68" s="2"/>
       <c r="H68" s="2"/>
       <c r="I68" s="2"/>
       <c r="J68" s="2"/>
@@ -3153,12 +3366,21 @@
       <c r="Z68" s="2"/>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
-      <c r="D69" s="2"/>
-      <c r="E69" s="2"/>
+      <c r="A69" s="7" t="n">
+        <v>68</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D69" s="7"/>
+      <c r="E69" s="7" t="n">
+        <f aca="false">A65</f>
+        <v>64</v>
+      </c>
       <c r="F69" s="2"/>
-      <c r="G69" s="2"/>
       <c r="H69" s="2"/>
       <c r="I69" s="2"/>
       <c r="J69" s="2"/>
@@ -3180,12 +3402,23 @@
       <c r="Z69" s="2"/>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="2"/>
-      <c r="C70" s="2"/>
-      <c r="D70" s="2"/>
-      <c r="E70" s="2"/>
+      <c r="A70" s="7" t="n">
+        <v>69</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D70" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E70" s="7" t="n">
+        <f aca="false">A69</f>
+        <v>68</v>
+      </c>
       <c r="F70" s="2"/>
-      <c r="G70" s="2"/>
       <c r="H70" s="2"/>
       <c r="I70" s="2"/>
       <c r="J70" s="2"/>
@@ -3207,12 +3440,23 @@
       <c r="Z70" s="2"/>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="2"/>
-      <c r="C71" s="2"/>
-      <c r="D71" s="2"/>
-      <c r="E71" s="2"/>
+      <c r="A71" s="7" t="n">
+        <v>70</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D71" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E71" s="7" t="n">
+        <f aca="false">A65</f>
+        <v>64</v>
+      </c>
       <c r="F71" s="2"/>
-      <c r="G71" s="2"/>
       <c r="H71" s="2"/>
       <c r="I71" s="2"/>
       <c r="J71" s="2"/>
@@ -3234,12 +3478,21 @@
       <c r="Z71" s="2"/>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="2"/>
-      <c r="C72" s="2"/>
-      <c r="D72" s="2"/>
-      <c r="E72" s="2"/>
+      <c r="A72" s="7" t="n">
+        <v>71</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D72" s="7"/>
+      <c r="E72" s="7" t="n">
+        <f aca="false">A64</f>
+        <v>63</v>
+      </c>
       <c r="F72" s="2"/>
-      <c r="G72" s="2"/>
       <c r="H72" s="2"/>
       <c r="I72" s="2"/>
       <c r="J72" s="2"/>
@@ -3261,12 +3514,21 @@
       <c r="Z72" s="2"/>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="2"/>
-      <c r="C73" s="2"/>
-      <c r="D73" s="2"/>
-      <c r="E73" s="2"/>
+      <c r="A73" s="7" t="n">
+        <v>72</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D73" s="7"/>
+      <c r="E73" s="7" t="n">
+        <f aca="false">A72</f>
+        <v>71</v>
+      </c>
       <c r="F73" s="2"/>
-      <c r="G73" s="2"/>
       <c r="H73" s="2"/>
       <c r="I73" s="2"/>
       <c r="J73" s="2"/>
@@ -3288,12 +3550,23 @@
       <c r="Z73" s="2"/>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="2"/>
-      <c r="C74" s="2"/>
-      <c r="D74" s="2"/>
-      <c r="E74" s="2"/>
+      <c r="A74" s="7" t="n">
+        <v>73</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D74" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E74" s="7" t="n">
+        <f aca="false">A73</f>
+        <v>72</v>
+      </c>
       <c r="F74" s="2"/>
-      <c r="G74" s="2"/>
       <c r="H74" s="2"/>
       <c r="I74" s="2"/>
       <c r="J74" s="2"/>
@@ -3315,12 +3588,23 @@
       <c r="Z74" s="2"/>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="2"/>
-      <c r="C75" s="2"/>
-      <c r="D75" s="2"/>
-      <c r="E75" s="2"/>
+      <c r="A75" s="7" t="n">
+        <v>74</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C75" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E75" s="7" t="n">
+        <f aca="false">A73</f>
+        <v>72</v>
+      </c>
       <c r="F75" s="2"/>
-      <c r="G75" s="2"/>
       <c r="H75" s="2"/>
       <c r="I75" s="2"/>
       <c r="J75" s="2"/>
@@ -3342,12 +3626,23 @@
       <c r="Z75" s="2"/>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="2"/>
-      <c r="C76" s="2"/>
-      <c r="D76" s="2"/>
-      <c r="E76" s="2"/>
+      <c r="A76" s="7" t="n">
+        <v>75</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D76" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E76" s="7" t="n">
+        <f aca="false">A72</f>
+        <v>71</v>
+      </c>
       <c r="F76" s="2"/>
-      <c r="G76" s="2"/>
       <c r="H76" s="2"/>
       <c r="I76" s="2"/>
       <c r="J76" s="2"/>
@@ -3368,13 +3663,24 @@
       <c r="Y76" s="2"/>
       <c r="Z76" s="2"/>
     </row>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B77" s="2"/>
-      <c r="C77" s="2"/>
-      <c r="D77" s="2"/>
-      <c r="E77" s="2"/>
+    <row r="77" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="7" t="n">
+        <v>76</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D77" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E77" s="7" t="n">
+        <f aca="false">A53</f>
+        <v>52</v>
+      </c>
       <c r="F77" s="2"/>
-      <c r="G77" s="2"/>
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
       <c r="J77" s="2"/>
@@ -3396,12 +3702,21 @@
       <c r="Z77" s="2"/>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B78" s="2"/>
-      <c r="C78" s="2"/>
-      <c r="D78" s="2"/>
-      <c r="E78" s="2"/>
+      <c r="A78" s="7" t="n">
+        <v>77</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D78" s="7"/>
+      <c r="E78" s="7" t="n">
+        <f aca="false">A77</f>
+        <v>76</v>
+      </c>
       <c r="F78" s="2"/>
-      <c r="G78" s="2"/>
       <c r="H78" s="2"/>
       <c r="I78" s="2"/>
       <c r="J78" s="2"/>
@@ -3422,13 +3737,24 @@
       <c r="Y78" s="2"/>
       <c r="Z78" s="2"/>
     </row>
-    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B79" s="2"/>
-      <c r="C79" s="2"/>
-      <c r="D79" s="2"/>
-      <c r="E79" s="2"/>
+    <row r="79" customFormat="false" ht="173.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="7" t="n">
+        <v>78</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D79" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E79" s="7" t="n">
+        <f aca="false">A78</f>
+        <v>77</v>
+      </c>
       <c r="F79" s="2"/>
-      <c r="G79" s="2"/>
       <c r="H79" s="2"/>
       <c r="I79" s="2"/>
       <c r="J79" s="2"/>
@@ -3449,13 +3775,24 @@
       <c r="Y79" s="2"/>
       <c r="Z79" s="2"/>
     </row>
-    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
-      <c r="D80" s="2"/>
-      <c r="E80" s="2"/>
+    <row r="80" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="7" t="n">
+        <v>79</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D80" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E80" s="7" t="n">
+        <f aca="false">A78</f>
+        <v>77</v>
+      </c>
       <c r="F80" s="2"/>
-      <c r="G80" s="2"/>
       <c r="H80" s="2"/>
       <c r="I80" s="2"/>
       <c r="J80" s="2"/>
@@ -3476,13 +3813,24 @@
       <c r="Y80" s="2"/>
       <c r="Z80" s="2"/>
     </row>
-    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B81" s="2"/>
-      <c r="C81" s="2"/>
-      <c r="D81" s="2"/>
-      <c r="E81" s="2"/>
+    <row r="81" customFormat="false" ht="127.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="7" t="n">
+        <v>80</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D81" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="E81" s="7" t="n">
+        <f aca="false">A78</f>
+        <v>77</v>
+      </c>
       <c r="F81" s="2"/>
-      <c r="G81" s="2"/>
       <c r="H81" s="2"/>
       <c r="I81" s="2"/>
       <c r="J81" s="2"/>
@@ -3504,12 +3852,23 @@
       <c r="Z81" s="2"/>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="2"/>
-      <c r="C82" s="2"/>
-      <c r="D82" s="2"/>
-      <c r="E82" s="2"/>
+      <c r="A82" s="7" t="n">
+        <v>81</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D82" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E82" s="7" t="n">
+        <f aca="false">A53</f>
+        <v>52</v>
+      </c>
       <c r="F82" s="2"/>
-      <c r="G82" s="2"/>
       <c r="H82" s="2"/>
       <c r="I82" s="2"/>
       <c r="J82" s="2"/>
@@ -3531,12 +3890,23 @@
       <c r="Z82" s="2"/>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B83" s="2"/>
-      <c r="C83" s="2"/>
-      <c r="D83" s="2"/>
-      <c r="E83" s="2"/>
+      <c r="A83" s="7" t="n">
+        <v>82</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D83" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E83" s="7" t="n">
+        <f aca="false">A82</f>
+        <v>81</v>
+      </c>
       <c r="F83" s="2"/>
-      <c r="G83" s="2"/>
       <c r="H83" s="2"/>
       <c r="I83" s="2"/>
       <c r="J83" s="2"/>
@@ -3557,13 +3927,24 @@
       <c r="Y83" s="2"/>
       <c r="Z83" s="2"/>
     </row>
-    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="2"/>
-      <c r="C84" s="2"/>
-      <c r="D84" s="2"/>
-      <c r="E84" s="2"/>
+    <row r="84" customFormat="false" ht="92.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="7" t="n">
+        <v>83</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="D84" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E84" s="7" t="n">
+        <f aca="false">A83</f>
+        <v>82</v>
+      </c>
       <c r="F84" s="2"/>
-      <c r="G84" s="2"/>
       <c r="H84" s="2"/>
       <c r="I84" s="2"/>
       <c r="J84" s="2"/>
@@ -3584,13 +3965,24 @@
       <c r="Y84" s="2"/>
       <c r="Z84" s="2"/>
     </row>
-    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B85" s="2"/>
-      <c r="C85" s="2"/>
-      <c r="D85" s="2"/>
-      <c r="E85" s="2"/>
+    <row r="85" customFormat="false" ht="81.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="7" t="n">
+        <v>84</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D85" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E85" s="7" t="n">
+        <f aca="false">A83</f>
+        <v>82</v>
+      </c>
       <c r="F85" s="2"/>
-      <c r="G85" s="2"/>
       <c r="H85" s="2"/>
       <c r="I85" s="2"/>
       <c r="J85" s="2"/>
@@ -3611,13 +4003,24 @@
       <c r="Y85" s="2"/>
       <c r="Z85" s="2"/>
     </row>
-    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B86" s="2"/>
-      <c r="C86" s="2"/>
-      <c r="D86" s="2"/>
-      <c r="E86" s="2"/>
+    <row r="86" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="7" t="n">
+        <v>85</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D86" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E86" s="7" t="n">
+        <f aca="false">A83</f>
+        <v>82</v>
+      </c>
       <c r="F86" s="2"/>
-      <c r="G86" s="2"/>
       <c r="H86" s="2"/>
       <c r="I86" s="2"/>
       <c r="J86" s="2"/>
@@ -3639,12 +4042,23 @@
       <c r="Z86" s="2"/>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B87" s="2"/>
-      <c r="C87" s="2"/>
-      <c r="D87" s="2"/>
-      <c r="E87" s="2"/>
+      <c r="A87" s="7" t="n">
+        <v>86</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D87" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E87" s="7" t="n">
+        <f aca="false">A82</f>
+        <v>81</v>
+      </c>
       <c r="F87" s="2"/>
-      <c r="G87" s="2"/>
       <c r="H87" s="2"/>
       <c r="I87" s="2"/>
       <c r="J87" s="2"/>
@@ -3666,12 +4080,23 @@
       <c r="Z87" s="2"/>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B88" s="2"/>
-      <c r="C88" s="2"/>
-      <c r="D88" s="2"/>
-      <c r="E88" s="2"/>
+      <c r="A88" s="7" t="n">
+        <v>87</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D88" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E88" s="7" t="n">
+        <f aca="false">A87</f>
+        <v>86</v>
+      </c>
       <c r="F88" s="2"/>
-      <c r="G88" s="2"/>
       <c r="H88" s="2"/>
       <c r="I88" s="2"/>
       <c r="J88" s="2"/>
@@ -3692,13 +4117,24 @@
       <c r="Y88" s="2"/>
       <c r="Z88" s="2"/>
     </row>
-    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B89" s="2"/>
-      <c r="C89" s="2"/>
-      <c r="D89" s="2"/>
-      <c r="E89" s="2"/>
+    <row r="89" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="7" t="n">
+        <v>88</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C89" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D89" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E89" s="7" t="n">
+        <f aca="false">A88</f>
+        <v>87</v>
+      </c>
       <c r="F89" s="2"/>
-      <c r="G89" s="2"/>
       <c r="H89" s="2"/>
       <c r="I89" s="2"/>
       <c r="J89" s="2"/>
@@ -3720,12 +4156,21 @@
       <c r="Z89" s="2"/>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B90" s="2"/>
-      <c r="C90" s="2"/>
-      <c r="D90" s="2"/>
-      <c r="E90" s="2"/>
+      <c r="A90" s="7" t="n">
+        <v>89</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C90" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D90" s="7"/>
+      <c r="E90" s="7" t="n">
+        <f aca="false">A82</f>
+        <v>81</v>
+      </c>
       <c r="F90" s="2"/>
-      <c r="G90" s="2"/>
       <c r="H90" s="2"/>
       <c r="I90" s="2"/>
       <c r="J90" s="2"/>
@@ -3747,12 +4192,23 @@
       <c r="Z90" s="2"/>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B91" s="2"/>
-      <c r="C91" s="2"/>
-      <c r="D91" s="2"/>
-      <c r="E91" s="2"/>
+      <c r="A91" s="7" t="n">
+        <v>90</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C91" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D91" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E91" s="7" t="n">
+        <f aca="false">A90</f>
+        <v>89</v>
+      </c>
       <c r="F91" s="2"/>
-      <c r="G91" s="2"/>
       <c r="H91" s="2"/>
       <c r="I91" s="2"/>
       <c r="J91" s="2"/>
@@ -3774,12 +4230,23 @@
       <c r="Z91" s="2"/>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B92" s="2"/>
-      <c r="C92" s="2"/>
-      <c r="D92" s="2"/>
-      <c r="E92" s="2"/>
+      <c r="A92" s="7" t="n">
+        <v>91</v>
+      </c>
+      <c r="B92" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D92" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E92" s="7" t="n">
+        <f aca="false">A90</f>
+        <v>89</v>
+      </c>
       <c r="F92" s="2"/>
-      <c r="G92" s="2"/>
       <c r="H92" s="2"/>
       <c r="I92" s="2"/>
       <c r="J92" s="2"/>
@@ -3800,13 +4267,24 @@
       <c r="Y92" s="2"/>
       <c r="Z92" s="2"/>
     </row>
-    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B93" s="2"/>
-      <c r="C93" s="2"/>
-      <c r="D93" s="2"/>
-      <c r="E93" s="2"/>
+    <row r="93" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="7" t="n">
+        <v>92</v>
+      </c>
+      <c r="B93" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C93" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D93" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="E93" s="7" t="n">
+        <f aca="false">A90</f>
+        <v>89</v>
+      </c>
       <c r="F93" s="2"/>
-      <c r="G93" s="2"/>
       <c r="H93" s="2"/>
       <c r="I93" s="2"/>
       <c r="J93" s="2"/>
@@ -3827,13 +4305,24 @@
       <c r="Y93" s="2"/>
       <c r="Z93" s="2"/>
     </row>
-    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B94" s="2"/>
-      <c r="C94" s="2"/>
-      <c r="D94" s="2"/>
-      <c r="E94" s="2"/>
+    <row r="94" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="7" t="n">
+        <v>93</v>
+      </c>
+      <c r="B94" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C94" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D94" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="E94" s="7" t="n">
+        <f aca="false">A90</f>
+        <v>89</v>
+      </c>
       <c r="F94" s="2"/>
-      <c r="G94" s="2"/>
       <c r="H94" s="2"/>
       <c r="I94" s="2"/>
       <c r="J94" s="2"/>
@@ -3855,12 +4344,22 @@
       <c r="Z94" s="2"/>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B95" s="2"/>
-      <c r="C95" s="2"/>
-      <c r="D95" s="2"/>
-      <c r="E95" s="2"/>
-      <c r="F95" s="2"/>
-      <c r="G95" s="2"/>
+      <c r="A95" s="7" t="n">
+        <v>94</v>
+      </c>
+      <c r="B95" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C95" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D95" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E95" s="7"/>
+      <c r="F95" s="2" t="s">
+        <v>82</v>
+      </c>
       <c r="H95" s="2"/>
       <c r="I95" s="2"/>
       <c r="J95" s="2"/>
@@ -3881,13 +4380,24 @@
       <c r="Y95" s="2"/>
       <c r="Z95" s="2"/>
     </row>
-    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B96" s="2"/>
-      <c r="C96" s="2"/>
-      <c r="D96" s="2"/>
-      <c r="E96" s="2"/>
+    <row r="96" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="7" t="n">
+        <v>95</v>
+      </c>
+      <c r="B96" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C96" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D96" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E96" s="7" t="n">
+        <f aca="false">A95</f>
+        <v>94</v>
+      </c>
       <c r="F96" s="2"/>
-      <c r="G96" s="2"/>
       <c r="H96" s="2"/>
       <c r="I96" s="2"/>
       <c r="J96" s="2"/>
@@ -3909,12 +4419,23 @@
       <c r="Z96" s="2"/>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B97" s="2"/>
-      <c r="C97" s="2"/>
-      <c r="D97" s="2"/>
-      <c r="E97" s="2"/>
+      <c r="A97" s="7" t="n">
+        <v>96</v>
+      </c>
+      <c r="B97" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C97" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D97" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E97" s="7" t="n">
+        <f aca="false">A96</f>
+        <v>95</v>
+      </c>
       <c r="F97" s="2"/>
-      <c r="G97" s="2"/>
       <c r="H97" s="2"/>
       <c r="I97" s="2"/>
       <c r="J97" s="2"/>
@@ -3935,13 +4456,24 @@
       <c r="Y97" s="2"/>
       <c r="Z97" s="2"/>
     </row>
-    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B98" s="2"/>
-      <c r="C98" s="2"/>
-      <c r="D98" s="2"/>
-      <c r="E98" s="2"/>
+    <row r="98" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="7" t="n">
+        <v>97</v>
+      </c>
+      <c r="B98" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C98" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D98" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="E98" s="7" t="n">
+        <f aca="false">A97</f>
+        <v>96</v>
+      </c>
       <c r="F98" s="2"/>
-      <c r="G98" s="2"/>
       <c r="H98" s="2"/>
       <c r="I98" s="2"/>
       <c r="J98" s="2"/>
@@ -3962,11 +4494,23 @@
       <c r="Y98" s="2"/>
       <c r="Z98" s="2"/>
     </row>
-    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B99" s="2"/>
-      <c r="C99" s="2"/>
-      <c r="D99" s="2"/>
-      <c r="E99" s="2"/>
+    <row r="99" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="7" t="n">
+        <v>98</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C99" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D99" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="E99" s="7" t="n">
+        <f aca="false">A97</f>
+        <v>96</v>
+      </c>
       <c r="F99" s="2"/>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
@@ -3989,11 +4533,23 @@
       <c r="Y99" s="2"/>
       <c r="Z99" s="2"/>
     </row>
-    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B100" s="2"/>
-      <c r="C100" s="2"/>
-      <c r="D100" s="2"/>
-      <c r="E100" s="2"/>
+    <row r="100" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="7" t="n">
+        <v>99</v>
+      </c>
+      <c r="B100" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C100" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D100" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="E100" s="7" t="n">
+        <f aca="false">A97</f>
+        <v>96</v>
+      </c>
       <c r="F100" s="2"/>
       <c r="G100" s="2"/>
       <c r="H100" s="2"/>
@@ -4016,12 +4572,23 @@
       <c r="Y100" s="2"/>
       <c r="Z100" s="2"/>
     </row>
-    <row r="101" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="2"/>
-      <c r="B101" s="2"/>
-      <c r="C101" s="2"/>
-      <c r="D101" s="2"/>
-      <c r="E101" s="2"/>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="7" t="n">
+        <v>100</v>
+      </c>
+      <c r="B101" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C101" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D101" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="E101" s="7" t="n">
+        <f aca="false">A97</f>
+        <v>96</v>
+      </c>
       <c r="F101" s="2"/>
       <c r="G101" s="2"/>
       <c r="H101" s="2"/>
@@ -4044,12 +4611,23 @@
       <c r="Y101" s="2"/>
       <c r="Z101" s="2"/>
     </row>
-    <row r="102" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="2"/>
-      <c r="B102" s="2"/>
-      <c r="C102" s="2"/>
-      <c r="D102" s="2"/>
-      <c r="E102" s="2"/>
+    <row r="102" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="7" t="n">
+        <v>101</v>
+      </c>
+      <c r="B102" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C102" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="D102" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E102" s="7" t="n">
+        <f aca="false">A97</f>
+        <v>96</v>
+      </c>
       <c r="F102" s="2"/>
       <c r="G102" s="2"/>
       <c r="H102" s="2"/>
@@ -4072,12 +4650,23 @@
       <c r="Y102" s="2"/>
       <c r="Z102" s="2"/>
     </row>
-    <row r="103" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="2"/>
-      <c r="B103" s="2"/>
-      <c r="C103" s="2"/>
-      <c r="D103" s="2"/>
-      <c r="E103" s="2"/>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="7" t="n">
+        <v>102</v>
+      </c>
+      <c r="B103" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C103" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D103" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="E103" s="7" t="n">
+        <f aca="false">A96</f>
+        <v>95</v>
+      </c>
       <c r="F103" s="2"/>
       <c r="G103" s="2"/>
       <c r="H103" s="2"/>

</xml_diff>

<commit_message>
added Tag model to criteriaCatalog. Added import of Tag to data_import.py
</commit_message>
<xml_diff>
--- a/02_work_doc/01_daten/08_criteriaCatalog/Tabelle_Wissensplattform_criteriaCatalog_Personalisierung.xlsx
+++ b/02_work_doc/01_daten/08_criteriaCatalog/Tabelle_Wissensplattform_criteriaCatalog_Personalisierung.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="108">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -40,6 +40,16 @@
     <t xml:space="preserve">image</t>
   </si>
   <si>
+    <t xml:space="preserve">tags</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ueberschrift_en
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">text_en</t>
+  </si>
+  <si>
     <t xml:space="preserve">Profilbildung und Personalisierung</t>
   </si>
   <si>
@@ -52,13 +62,23 @@
     <t xml:space="preserve">data.svg</t>
   </si>
   <si>
+    <t xml:space="preserve">Personenbezug der Daten, Anwendungsbereich, Scope, Personenbezug, Personenbezogene Daten, Anonymisierung, Identifizierbarkeit, PID, PII, Personal Data, Personal Identifiable Data, Personal Identifiable Information</t>
+  </si>
+  <si>
     <t xml:space="preserve">Spezifikation der Datenkategorien</t>
   </si>
   <si>
     <t xml:space="preserve">Zunächst muss der Verantwortliche spezifizieren, welche Datenkategorien überhaupt verarbeitet werden.</t>
   </si>
   <si>
+    <t xml:space="preserve">Daten, Spezifikation, Art der Daten, Datenarten
+Datenkategorien</t>
+  </si>
+  <si>
     <t xml:space="preserve">Es werden ausschließlich Raumklimadaten, Gebäudedaten und Energie-Verbrauchsdaten verarbeitet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raumklima, Gebäude, Verbrauch, Messdaten, CO2, Temperatur, Feuchte, VOC</t>
   </si>
   <si>
     <t xml:space="preserve">a) Raumklimadaten</t>
@@ -142,6 +162,9 @@
   <si>
     <t xml:space="preserve">Anknüpfungspunkt für jeden datenschutzrechtliche Prüfung ist die Frage, ob in einem Verarbeitungsvorgang "personenbezogene Daten" verarbeitet werden und damit der Anwendungsbereich der Datenschutz-Grundverordnung (DSGVO) eröffnet ist. Aufgrund der sehr weiten Legaldefinition aus Art. 4 Nr. 1 DSGVO ist eine pauschale Beantwortung diese Frage kaum möglich, da auch rein technische Daten mit Personen verknüpft werden können. Ob Daten im konkreten Fall personenbezogen oder nicht, kann anhand der folgenden Kriterien ermittelt werden. In diesem ersten Kriterium wird überprüft, ob die verarbeiteten Daten schon aufgrund ihres Inhalts (und unabhängig vom konkreten Verarbeitungszweck) Personebezug aufweisen. Das ist der Fall, wenn der Informationsgehalt der Daten dem abgeschirmten, privaten Lebensbereich einer Person zuzuordnen ist, unabhängig davon wie und wofür die Daten verarbeitet werden (Inhaltselement).
 Hiermit verknüpft ist die Frage, ob die davon betroffnen Personen auch "identifizierbar" sind iSv. Art. 4 Nr. 1 DSGVO . Wann eine Person identifiziert ist, unterscheidet sich wieder grundsätzlich nach der jeweils betroffenen Sphäre des Privatlebens. Im vorliegenden Szenario wird eine Identifizierbarkeit der Personen vermutet, da eine Rückführung von gebäudespezifischen Daten auf eine einzelne Person über Telefonbücher, Klingelschilder, Grundbuch, Raumbelegungspläne und sonstigen Quellen üblicherweise möglich ist oder zumindest nicht ausgeschlossen werden kann.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inhaltselement, About Element, Personenbezug, Inhalt</t>
   </si>
   <si>
     <t xml:space="preserve">Es wurde spezifiziert, welche Daten bereits aufgrund ihres Inhalts personenbezogen sind</t>
@@ -455,7 +478,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -480,6 +503,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
@@ -564,7 +594,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -577,11 +607,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -589,7 +627,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -601,7 +643,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -609,7 +651,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -752,10 +794,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.62"/>
@@ -763,7 +805,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="6.62"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="40.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -782,9 +824,15 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
@@ -808,19 +856,21 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
@@ -841,25 +891,27 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="73.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E3" s="2" t="n">
         <f aca="false">A2</f>
         <v>1</v>
       </c>
       <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="G3" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -885,10 +937,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="n">
@@ -896,7 +948,9 @@
         <v>2</v>
       </c>
       <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -922,13 +976,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E5" s="2" t="n">
         <f aca="false">A4</f>
@@ -961,13 +1015,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E6" s="2" t="n">
         <f aca="false">A4</f>
@@ -1000,13 +1054,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="E7" s="2" t="n">
         <f aca="false">A4</f>
@@ -1039,10 +1093,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="n">
@@ -1076,13 +1130,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>21</v>
+        <v>26</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="E9" s="2" t="n">
         <f aca="false">A8</f>
@@ -1115,20 +1169,23 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>23</v>
+        <v>9</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="E10" s="2" t="n">
         <f aca="false">A8</f>
         <v>7</v>
       </c>
       <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" s="8"/>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
@@ -1153,20 +1210,23 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>25</v>
+        <v>9</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="E11" s="2" t="n">
         <f aca="false">A8</f>
         <v>7</v>
       </c>
       <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="8"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -1191,20 +1251,22 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>27</v>
+        <v>32</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="E12" s="2" t="n">
         <f aca="false">A2</f>
         <v>1</v>
       </c>
       <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -1230,10 +1292,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="n">
@@ -1267,10 +1329,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="n">
@@ -1304,10 +1366,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2" t="n">
@@ -1341,13 +1403,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>32</v>
+        <v>38</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="E16" s="2" t="n">
         <f aca="false">A15</f>
@@ -1380,13 +1442,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>33</v>
+        <v>9</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>40</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="E17" s="2" t="n">
         <f aca="false">A15</f>
@@ -1419,10 +1481,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2" t="n">
@@ -1456,13 +1518,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="E19" s="2" t="n">
         <f aca="false">A18</f>
@@ -1495,13 +1557,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="E20" s="2" t="n">
         <f aca="false">A14</f>
@@ -1534,10 +1596,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2" t="n">
@@ -1571,10 +1633,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2" t="n">
@@ -1608,13 +1670,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="E23" s="2" t="n">
         <f aca="false">A22</f>
@@ -1647,13 +1709,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>43</v>
+        <v>9</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>50</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="E24" s="2" t="n">
         <f aca="false">A22</f>
@@ -1686,13 +1748,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="E25" s="2" t="n">
         <f aca="false">A21</f>
@@ -1725,13 +1787,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>48</v>
+        <v>54</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="E26" s="2" t="n">
         <f aca="false">A2</f>
@@ -1764,10 +1826,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2" t="n">
@@ -1801,13 +1863,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>51</v>
+        <v>57</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="E28" s="2" t="n">
         <f aca="false">A27</f>
@@ -1840,13 +1902,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>53</v>
+        <v>59</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>60</v>
       </c>
       <c r="E29" s="2" t="n">
         <f aca="false">A27</f>
@@ -1879,13 +1941,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>55</v>
+        <v>61</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>62</v>
       </c>
       <c r="E30" s="2" t="n">
         <f aca="false">A27</f>
@@ -1918,13 +1980,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="E31" s="2" t="n">
         <f aca="false">A2</f>
@@ -1957,13 +2019,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="E32" s="2" t="n">
         <f aca="false">A31</f>
@@ -1996,13 +2058,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>61</v>
+        <v>67</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>68</v>
       </c>
       <c r="E33" s="2" t="n">
         <f aca="false">A32</f>
@@ -2035,13 +2097,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>63</v>
+        <v>69</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="E34" s="2" t="n">
         <f aca="false">A32</f>
@@ -2074,13 +2136,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>65</v>
+        <v>71</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>72</v>
       </c>
       <c r="E35" s="2" t="n">
         <f aca="false">A32</f>
@@ -2113,13 +2175,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="E36" s="2" t="n">
         <f aca="false">A31</f>
@@ -2152,13 +2214,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="E37" s="2" t="n">
         <f aca="false">A36</f>
@@ -2191,13 +2253,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>71</v>
+        <v>77</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="E38" s="2" t="n">
         <f aca="false">A37</f>
@@ -2230,10 +2292,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2" t="n">
@@ -2267,13 +2329,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="E40" s="2" t="n">
         <f aca="false">A39</f>
@@ -2306,13 +2368,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="E41" s="2" t="n">
         <f aca="false">A39</f>
@@ -2345,13 +2407,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>77</v>
+        <v>83</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="E42" s="2" t="n">
         <f aca="false">A39</f>
@@ -2384,13 +2446,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>79</v>
+        <v>85</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="E43" s="2" t="n">
         <f aca="false">A39</f>
@@ -2423,17 +2485,17 @@
         <v>43</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="2" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
@@ -2461,13 +2523,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>84</v>
+        <v>90</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>91</v>
       </c>
       <c r="E45" s="2" t="n">
         <f aca="false">A44</f>
@@ -2500,13 +2562,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="E46" s="2" t="n">
         <f aca="false">A45</f>
@@ -2539,13 +2601,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>88</v>
+        <v>94</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>95</v>
       </c>
       <c r="E47" s="2" t="n">
         <f aca="false">A46</f>
@@ -2578,13 +2640,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>90</v>
+        <v>96</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>97</v>
       </c>
       <c r="E48" s="2" t="n">
         <f aca="false">A46</f>
@@ -2617,13 +2679,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>92</v>
+        <v>98</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>99</v>
       </c>
       <c r="E49" s="2" t="n">
         <f aca="false">A46</f>
@@ -2656,13 +2718,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="E50" s="2" t="n">
         <f aca="false">A46</f>
@@ -2695,13 +2757,13 @@
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>96</v>
+        <v>102</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>103</v>
       </c>
       <c r="E51" s="2" t="n">
         <f aca="false">A46</f>
@@ -2734,13 +2796,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="E52" s="2" t="n">
         <f aca="false">A45</f>
@@ -2769,21 +2831,21 @@
       <c r="Z52" s="2"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="7" t="n">
+      <c r="A53" s="10" t="n">
         <v>52</v>
       </c>
-      <c r="B53" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D53" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E53" s="7"/>
+      <c r="B53" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E53" s="10"/>
       <c r="F53" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
@@ -2806,19 +2868,19 @@
       <c r="Z53" s="2"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="7" t="n">
+      <c r="A54" s="10" t="n">
         <v>53</v>
       </c>
-      <c r="B54" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C54" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D54" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="E54" s="7" t="n">
+      <c r="B54" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E54" s="10" t="n">
         <f aca="false">A53</f>
         <v>52</v>
       </c>
@@ -2844,17 +2906,17 @@
       <c r="Z54" s="2"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="7" t="n">
+      <c r="A55" s="10" t="n">
         <v>54</v>
       </c>
-      <c r="B55" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C55" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D55" s="7"/>
-      <c r="E55" s="7" t="n">
+      <c r="B55" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D55" s="10"/>
+      <c r="E55" s="10" t="n">
         <f aca="false">A54</f>
         <v>53</v>
       </c>
@@ -2880,19 +2942,19 @@
       <c r="Z55" s="2"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="7" t="n">
+      <c r="A56" s="10" t="n">
         <v>55</v>
       </c>
-      <c r="B56" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C56" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D56" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E56" s="7" t="n">
+      <c r="B56" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C56" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E56" s="10" t="n">
         <f aca="false">A55</f>
         <v>54</v>
       </c>
@@ -2918,19 +2980,19 @@
       <c r="Z56" s="2"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="7" t="n">
+      <c r="A57" s="10" t="n">
         <v>56</v>
       </c>
-      <c r="B57" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C57" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D57" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E57" s="7" t="n">
+      <c r="B57" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C57" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E57" s="10" t="n">
         <f aca="false">A55</f>
         <v>54</v>
       </c>
@@ -2956,19 +3018,19 @@
       <c r="Z57" s="2"/>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="7" t="n">
+      <c r="A58" s="10" t="n">
         <v>57</v>
       </c>
-      <c r="B58" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C58" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D58" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E58" s="7" t="n">
+      <c r="B58" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C58" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D58" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E58" s="10" t="n">
         <f aca="false">A55</f>
         <v>54</v>
       </c>
@@ -2994,17 +3056,17 @@
       <c r="Z58" s="2"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="7" t="n">
+      <c r="A59" s="10" t="n">
         <v>58</v>
       </c>
-      <c r="B59" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C59" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D59" s="7"/>
-      <c r="E59" s="7" t="n">
+      <c r="B59" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D59" s="10"/>
+      <c r="E59" s="10" t="n">
         <f aca="false">A55</f>
         <v>54</v>
       </c>
@@ -3030,19 +3092,19 @@
       <c r="Z59" s="2"/>
     </row>
     <row r="60" customFormat="false" ht="173.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="7" t="n">
+      <c r="A60" s="10" t="n">
         <v>59</v>
       </c>
-      <c r="B60" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C60" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D60" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E60" s="7" t="n">
+      <c r="B60" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C60" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D60" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E60" s="10" t="n">
         <f aca="false">A59</f>
         <v>58</v>
       </c>
@@ -3068,19 +3130,19 @@
       <c r="Z60" s="2"/>
     </row>
     <row r="61" customFormat="false" ht="276.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="7" t="n">
+      <c r="A61" s="10" t="n">
         <v>60</v>
       </c>
-      <c r="B61" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C61" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D61" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="E61" s="7" t="n">
+      <c r="B61" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C61" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D61" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="E61" s="10" t="n">
         <f aca="false">A59</f>
         <v>58</v>
       </c>
@@ -3106,19 +3168,19 @@
       <c r="Z61" s="2"/>
     </row>
     <row r="62" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="7" t="n">
+      <c r="A62" s="10" t="n">
         <v>61</v>
       </c>
-      <c r="B62" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C62" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D62" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E62" s="7" t="n">
+      <c r="B62" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C62" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D62" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E62" s="10" t="n">
         <f aca="false">A59</f>
         <v>58</v>
       </c>
@@ -3144,19 +3206,19 @@
       <c r="Z62" s="2"/>
     </row>
     <row r="63" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="7" t="n">
+      <c r="A63" s="10" t="n">
         <v>62</v>
       </c>
-      <c r="B63" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C63" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D63" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E63" s="7" t="n">
+      <c r="B63" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C63" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D63" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E63" s="10" t="n">
         <f aca="false">A53</f>
         <v>52</v>
       </c>
@@ -3182,17 +3244,17 @@
       <c r="Z63" s="2"/>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="7" t="n">
+      <c r="A64" s="10" t="n">
         <v>63</v>
       </c>
-      <c r="B64" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C64" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D64" s="7"/>
-      <c r="E64" s="7" t="n">
+      <c r="B64" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C64" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D64" s="10"/>
+      <c r="E64" s="10" t="n">
         <f aca="false">A63</f>
         <v>62</v>
       </c>
@@ -3218,17 +3280,17 @@
       <c r="Z64" s="2"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="7" t="n">
+      <c r="A65" s="10" t="n">
         <v>64</v>
       </c>
-      <c r="B65" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C65" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D65" s="7"/>
-      <c r="E65" s="7" t="n">
+      <c r="B65" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C65" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D65" s="10"/>
+      <c r="E65" s="10" t="n">
         <f aca="false">A64</f>
         <v>63</v>
       </c>
@@ -3254,17 +3316,17 @@
       <c r="Z65" s="2"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="7" t="n">
+      <c r="A66" s="10" t="n">
         <v>65</v>
       </c>
-      <c r="B66" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C66" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D66" s="7"/>
-      <c r="E66" s="7" t="n">
+      <c r="B66" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C66" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D66" s="10"/>
+      <c r="E66" s="10" t="n">
         <f aca="false">A65</f>
         <v>64</v>
       </c>
@@ -3290,19 +3352,19 @@
       <c r="Z66" s="2"/>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="7" t="n">
+      <c r="A67" s="10" t="n">
         <v>66</v>
       </c>
-      <c r="B67" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C67" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D67" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E67" s="7" t="n">
+      <c r="B67" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C67" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D67" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E67" s="10" t="n">
         <f aca="false">A66</f>
         <v>65</v>
       </c>
@@ -3328,19 +3390,19 @@
       <c r="Z67" s="2"/>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="7" t="n">
+      <c r="A68" s="10" t="n">
         <v>67</v>
       </c>
-      <c r="B68" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C68" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D68" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E68" s="7" t="n">
+      <c r="B68" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C68" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D68" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E68" s="10" t="n">
         <f aca="false">A66</f>
         <v>65</v>
       </c>
@@ -3366,17 +3428,17 @@
       <c r="Z68" s="2"/>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="7" t="n">
+      <c r="A69" s="10" t="n">
         <v>68</v>
       </c>
-      <c r="B69" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C69" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D69" s="7"/>
-      <c r="E69" s="7" t="n">
+      <c r="B69" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C69" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="D69" s="10"/>
+      <c r="E69" s="10" t="n">
         <f aca="false">A65</f>
         <v>64</v>
       </c>
@@ -3402,19 +3464,19 @@
       <c r="Z69" s="2"/>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="7" t="n">
+      <c r="A70" s="10" t="n">
         <v>69</v>
       </c>
-      <c r="B70" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C70" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D70" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E70" s="7" t="n">
+      <c r="B70" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C70" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D70" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E70" s="10" t="n">
         <f aca="false">A69</f>
         <v>68</v>
       </c>
@@ -3440,19 +3502,19 @@
       <c r="Z70" s="2"/>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="7" t="n">
+      <c r="A71" s="10" t="n">
         <v>70</v>
       </c>
-      <c r="B71" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C71" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D71" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E71" s="7" t="n">
+      <c r="B71" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C71" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D71" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E71" s="10" t="n">
         <f aca="false">A65</f>
         <v>64</v>
       </c>
@@ -3478,17 +3540,17 @@
       <c r="Z71" s="2"/>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="7" t="n">
+      <c r="A72" s="10" t="n">
         <v>71</v>
       </c>
-      <c r="B72" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C72" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D72" s="7"/>
-      <c r="E72" s="7" t="n">
+      <c r="B72" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C72" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D72" s="10"/>
+      <c r="E72" s="10" t="n">
         <f aca="false">A64</f>
         <v>63</v>
       </c>
@@ -3514,17 +3576,17 @@
       <c r="Z72" s="2"/>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="7" t="n">
+      <c r="A73" s="10" t="n">
         <v>72</v>
       </c>
-      <c r="B73" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C73" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D73" s="7"/>
-      <c r="E73" s="7" t="n">
+      <c r="B73" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C73" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D73" s="10"/>
+      <c r="E73" s="10" t="n">
         <f aca="false">A72</f>
         <v>71</v>
       </c>
@@ -3550,19 +3612,19 @@
       <c r="Z73" s="2"/>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="7" t="n">
+      <c r="A74" s="10" t="n">
         <v>73</v>
       </c>
-      <c r="B74" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C74" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D74" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E74" s="7" t="n">
+      <c r="B74" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C74" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D74" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E74" s="10" t="n">
         <f aca="false">A73</f>
         <v>72</v>
       </c>
@@ -3588,19 +3650,19 @@
       <c r="Z74" s="2"/>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="7" t="n">
+      <c r="A75" s="10" t="n">
         <v>74</v>
       </c>
-      <c r="B75" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C75" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D75" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E75" s="7" t="n">
+      <c r="B75" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C75" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D75" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="E75" s="10" t="n">
         <f aca="false">A73</f>
         <v>72</v>
       </c>
@@ -3626,19 +3688,19 @@
       <c r="Z75" s="2"/>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="7" t="n">
+      <c r="A76" s="10" t="n">
         <v>75</v>
       </c>
-      <c r="B76" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C76" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D76" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E76" s="7" t="n">
+      <c r="B76" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C76" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D76" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E76" s="10" t="n">
         <f aca="false">A72</f>
         <v>71</v>
       </c>
@@ -3664,19 +3726,19 @@
       <c r="Z76" s="2"/>
     </row>
     <row r="77" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="7" t="n">
+      <c r="A77" s="10" t="n">
         <v>76</v>
       </c>
-      <c r="B77" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C77" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D77" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E77" s="7" t="n">
+      <c r="B77" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C77" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D77" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E77" s="10" t="n">
         <f aca="false">A53</f>
         <v>52</v>
       </c>
@@ -3702,17 +3764,17 @@
       <c r="Z77" s="2"/>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="7" t="n">
+      <c r="A78" s="10" t="n">
         <v>77</v>
       </c>
-      <c r="B78" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C78" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D78" s="7"/>
-      <c r="E78" s="7" t="n">
+      <c r="B78" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C78" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D78" s="10"/>
+      <c r="E78" s="10" t="n">
         <f aca="false">A77</f>
         <v>76</v>
       </c>
@@ -3738,19 +3800,19 @@
       <c r="Z78" s="2"/>
     </row>
     <row r="79" customFormat="false" ht="173.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="7" t="n">
+      <c r="A79" s="10" t="n">
         <v>78</v>
       </c>
-      <c r="B79" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C79" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D79" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E79" s="7" t="n">
+      <c r="B79" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C79" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D79" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E79" s="10" t="n">
         <f aca="false">A78</f>
         <v>77</v>
       </c>
@@ -3776,19 +3838,19 @@
       <c r="Z79" s="2"/>
     </row>
     <row r="80" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="7" t="n">
+      <c r="A80" s="10" t="n">
         <v>79</v>
       </c>
-      <c r="B80" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C80" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D80" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E80" s="7" t="n">
+      <c r="B80" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C80" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D80" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E80" s="10" t="n">
         <f aca="false">A78</f>
         <v>77</v>
       </c>
@@ -3814,19 +3876,19 @@
       <c r="Z80" s="2"/>
     </row>
     <row r="81" customFormat="false" ht="127.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="7" t="n">
+      <c r="A81" s="10" t="n">
         <v>80</v>
       </c>
-      <c r="B81" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C81" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D81" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E81" s="7" t="n">
+      <c r="B81" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C81" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D81" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E81" s="10" t="n">
         <f aca="false">A78</f>
         <v>77</v>
       </c>
@@ -3852,19 +3914,19 @@
       <c r="Z81" s="2"/>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="7" t="n">
+      <c r="A82" s="10" t="n">
         <v>81</v>
       </c>
-      <c r="B82" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C82" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D82" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="E82" s="7" t="n">
+      <c r="B82" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C82" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D82" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E82" s="10" t="n">
         <f aca="false">A53</f>
         <v>52</v>
       </c>
@@ -3890,19 +3952,19 @@
       <c r="Z82" s="2"/>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="7" t="n">
+      <c r="A83" s="10" t="n">
         <v>82</v>
       </c>
-      <c r="B83" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C83" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D83" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E83" s="7" t="n">
+      <c r="B83" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C83" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D83" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E83" s="10" t="n">
         <f aca="false">A82</f>
         <v>81</v>
       </c>
@@ -3928,19 +3990,19 @@
       <c r="Z83" s="2"/>
     </row>
     <row r="84" customFormat="false" ht="92.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="7" t="n">
+      <c r="A84" s="10" t="n">
         <v>83</v>
       </c>
-      <c r="B84" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C84" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D84" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="E84" s="7" t="n">
+      <c r="B84" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C84" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D84" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="E84" s="10" t="n">
         <f aca="false">A83</f>
         <v>82</v>
       </c>
@@ -3966,19 +4028,19 @@
       <c r="Z84" s="2"/>
     </row>
     <row r="85" customFormat="false" ht="81.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="7" t="n">
+      <c r="A85" s="10" t="n">
         <v>84</v>
       </c>
-      <c r="B85" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C85" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D85" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="E85" s="7" t="n">
+      <c r="B85" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C85" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D85" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E85" s="10" t="n">
         <f aca="false">A83</f>
         <v>82</v>
       </c>
@@ -4004,19 +4066,19 @@
       <c r="Z85" s="2"/>
     </row>
     <row r="86" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="7" t="n">
+      <c r="A86" s="10" t="n">
         <v>85</v>
       </c>
-      <c r="B86" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C86" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D86" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="E86" s="7" t="n">
+      <c r="B86" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C86" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D86" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="E86" s="10" t="n">
         <f aca="false">A83</f>
         <v>82</v>
       </c>
@@ -4042,19 +4104,19 @@
       <c r="Z86" s="2"/>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="7" t="n">
+      <c r="A87" s="10" t="n">
         <v>86</v>
       </c>
-      <c r="B87" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C87" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D87" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E87" s="7" t="n">
+      <c r="B87" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C87" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D87" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E87" s="10" t="n">
         <f aca="false">A82</f>
         <v>81</v>
       </c>
@@ -4080,19 +4142,19 @@
       <c r="Z87" s="2"/>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="7" t="n">
+      <c r="A88" s="10" t="n">
         <v>87</v>
       </c>
-      <c r="B88" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C88" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D88" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E88" s="7" t="n">
+      <c r="B88" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C88" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D88" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="E88" s="10" t="n">
         <f aca="false">A87</f>
         <v>86</v>
       </c>
@@ -4118,19 +4180,19 @@
       <c r="Z88" s="2"/>
     </row>
     <row r="89" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="7" t="n">
+      <c r="A89" s="10" t="n">
         <v>88</v>
       </c>
-      <c r="B89" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C89" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D89" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="E89" s="7" t="n">
+      <c r="B89" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C89" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D89" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E89" s="10" t="n">
         <f aca="false">A88</f>
         <v>87</v>
       </c>
@@ -4156,17 +4218,17 @@
       <c r="Z89" s="2"/>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="7" t="n">
+      <c r="A90" s="10" t="n">
         <v>89</v>
       </c>
-      <c r="B90" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C90" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D90" s="7"/>
-      <c r="E90" s="7" t="n">
+      <c r="B90" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C90" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D90" s="10"/>
+      <c r="E90" s="10" t="n">
         <f aca="false">A82</f>
         <v>81</v>
       </c>
@@ -4192,19 +4254,19 @@
       <c r="Z90" s="2"/>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="7" t="n">
+      <c r="A91" s="10" t="n">
         <v>90</v>
       </c>
-      <c r="B91" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C91" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D91" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E91" s="7" t="n">
+      <c r="B91" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C91" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D91" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="E91" s="10" t="n">
         <f aca="false">A90</f>
         <v>89</v>
       </c>
@@ -4230,19 +4292,19 @@
       <c r="Z91" s="2"/>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="7" t="n">
+      <c r="A92" s="10" t="n">
         <v>91</v>
       </c>
-      <c r="B92" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C92" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="D92" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="E92" s="7" t="n">
+      <c r="B92" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C92" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D92" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E92" s="10" t="n">
         <f aca="false">A90</f>
         <v>89</v>
       </c>
@@ -4268,19 +4330,19 @@
       <c r="Z92" s="2"/>
     </row>
     <row r="93" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="7" t="n">
+      <c r="A93" s="10" t="n">
         <v>92</v>
       </c>
-      <c r="B93" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C93" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D93" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="E93" s="7" t="n">
+      <c r="B93" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C93" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D93" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="E93" s="10" t="n">
         <f aca="false">A90</f>
         <v>89</v>
       </c>
@@ -4306,19 +4368,19 @@
       <c r="Z93" s="2"/>
     </row>
     <row r="94" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="7" t="n">
+      <c r="A94" s="10" t="n">
         <v>93</v>
       </c>
-      <c r="B94" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C94" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D94" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="E94" s="7" t="n">
+      <c r="B94" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C94" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D94" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="E94" s="10" t="n">
         <f aca="false">A90</f>
         <v>89</v>
       </c>
@@ -4344,21 +4406,21 @@
       <c r="Z94" s="2"/>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="7" t="n">
+      <c r="A95" s="10" t="n">
         <v>94</v>
       </c>
-      <c r="B95" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C95" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="D95" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="E95" s="7"/>
+      <c r="B95" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C95" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="D95" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="E95" s="10"/>
       <c r="F95" s="2" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="H95" s="2"/>
       <c r="I95" s="2"/>
@@ -4381,19 +4443,19 @@
       <c r="Z95" s="2"/>
     </row>
     <row r="96" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="7" t="n">
+      <c r="A96" s="10" t="n">
         <v>95</v>
       </c>
-      <c r="B96" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C96" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="D96" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="E96" s="7" t="n">
+      <c r="B96" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C96" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="D96" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="E96" s="10" t="n">
         <f aca="false">A95</f>
         <v>94</v>
       </c>
@@ -4419,19 +4481,19 @@
       <c r="Z96" s="2"/>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="7" t="n">
+      <c r="A97" s="10" t="n">
         <v>96</v>
       </c>
-      <c r="B97" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C97" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D97" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="E97" s="7" t="n">
+      <c r="B97" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C97" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D97" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="E97" s="10" t="n">
         <f aca="false">A96</f>
         <v>95</v>
       </c>
@@ -4457,19 +4519,19 @@
       <c r="Z97" s="2"/>
     </row>
     <row r="98" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="7" t="n">
+      <c r="A98" s="10" t="n">
         <v>97</v>
       </c>
-      <c r="B98" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C98" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="D98" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="E98" s="7" t="n">
+      <c r="B98" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C98" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D98" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E98" s="10" t="n">
         <f aca="false">A97</f>
         <v>96</v>
       </c>
@@ -4495,19 +4557,19 @@
       <c r="Z98" s="2"/>
     </row>
     <row r="99" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="7" t="n">
+      <c r="A99" s="10" t="n">
         <v>98</v>
       </c>
-      <c r="B99" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C99" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D99" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="E99" s="7" t="n">
+      <c r="B99" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C99" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D99" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="E99" s="10" t="n">
         <f aca="false">A97</f>
         <v>96</v>
       </c>
@@ -4534,19 +4596,19 @@
       <c r="Z99" s="2"/>
     </row>
     <row r="100" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="7" t="n">
+      <c r="A100" s="10" t="n">
         <v>99</v>
       </c>
-      <c r="B100" s="7" t="s">
+      <c r="B100" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C100" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D100" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="C100" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="D100" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="E100" s="7" t="n">
+      <c r="E100" s="10" t="n">
         <f aca="false">A97</f>
         <v>96</v>
       </c>
@@ -4573,19 +4635,19 @@
       <c r="Z100" s="2"/>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="7" t="n">
+      <c r="A101" s="10" t="n">
         <v>100</v>
       </c>
-      <c r="B101" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C101" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="D101" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="E101" s="7" t="n">
+      <c r="B101" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C101" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D101" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="E101" s="10" t="n">
         <f aca="false">A97</f>
         <v>96</v>
       </c>
@@ -4612,19 +4674,19 @@
       <c r="Z101" s="2"/>
     </row>
     <row r="102" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="7" t="n">
+      <c r="A102" s="10" t="n">
         <v>101</v>
       </c>
-      <c r="B102" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C102" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="D102" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="E102" s="7" t="n">
+      <c r="B102" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C102" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D102" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="E102" s="10" t="n">
         <f aca="false">A97</f>
         <v>96</v>
       </c>
@@ -4651,19 +4713,19 @@
       <c r="Z102" s="2"/>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="7" t="n">
+      <c r="A103" s="10" t="n">
         <v>102</v>
       </c>
-      <c r="B103" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C103" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D103" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E103" s="7" t="n">
+      <c r="B103" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="C103" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="D103" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="E103" s="10" t="n">
         <f aca="false">A96</f>
         <v>95</v>
       </c>

</xml_diff>

<commit_message>
implemented first expanding feature for tags
</commit_message>
<xml_diff>
--- a/02_work_doc/01_daten/08_criteriaCatalog/Tabelle_Wissensplattform_criteriaCatalog_Personalisierung.xlsx
+++ b/02_work_doc/01_daten/08_criteriaCatalog/Tabelle_Wissensplattform_criteriaCatalog_Personalisierung.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="112">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -232,7 +232,13 @@
 2. der Zweck unmittelbar mit einem der Beeinträchtigung eines Grundrechts einhergeht, insbesondere weil diesee Beeinträchtigung gerade bezweckt ist oder notwendige Folge des intendierten Zwecks.</t>
   </si>
   <si>
+    <t xml:space="preserve">Level 1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Es wurde spezifiziert welche Daten aufgrund des konkreten Verarbeitungszwecks personenbezogen sind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level 2</t>
   </si>
   <si>
     <t xml:space="preserve">Die Daten werden nicht verarbeitet, um einzelne Personen oder Personengruppen zu bewerten oder zu beeinflussen</t>
@@ -248,6 +254,9 @@
 3. Eine Identifizierung von Einzelpersonen oder Personengruppen scheint zur Erreichung des konkreten Zwecks nach allgemeinem Ermessen nicht erforderlich.
 4. Der AS hat im Rahmen seines Datenminimierungskonzeptes technische und organisatorische Maßnahmen implementiert, die sicherstellen, dass innerhalb seines Einflussbereichs eine Verarbeitung der Daten zur Bewertung oder Beeinflussung von Personen nicht erfolgt. Zu diesem Einflussbereich zählt das gesamte Unternehmen des AS sowie alle in diesem Unternehmen tätigen Personen, sowie dritte Unternehmen mit denen der AS in Beziehung steht und die mit der Datenverarbeitung in Verbindung stehen - insbesondere Auftragsverarbeiter iSv. Art. 4 Nr. 8 DSGVO.
 Der Verantwortliche kann darüber hinaus auch andere Nachweise erbringen, um zu bewerten, ob die Daten zur Bewertung oder Beeinflussung von Personen erfolgen. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level 3</t>
   </si>
   <si>
     <t xml:space="preserve">Es ergeben sich auch keine zusätzlichen Offenlegungsrisiken aufgrund des konkreten Verarbeitungszwecks</t>
@@ -313,6 +322,9 @@
 a) Veröffentlichung der Daten oder Teilen der Daten an einen nicht vertrauenswürdigen Dritten
 b) Vorsätzliches oder fahrlässiges Fehlverhalten von Mitarbeiter*innen
 c) Falsch konfiguriertes Zugangs- und Berechtigungsmanagement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moin</t>
   </si>
   <si>
     <t xml:space="preserve">Aufteilung der Risiken in abstrakte und konkrete Risiken</t>
@@ -478,7 +490,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -529,6 +541,12 @@
       <name val="&quot;Arial&quot;"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
       <b val="true"/>
@@ -594,7 +612,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -635,6 +653,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -643,7 +665,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -651,7 +673,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -791,13 +813,13 @@
   </sheetPr>
   <dimension ref="A1:Z1007"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+      <selection pane="bottomLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.62"/>
@@ -1800,7 +1822,9 @@
         <v>1</v>
       </c>
       <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
+      <c r="G26" s="10" t="s">
+        <v>56</v>
+      </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
@@ -1829,7 +1853,7 @@
         <v>9</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2" t="n">
@@ -1837,7 +1861,9 @@
         <v>25</v>
       </c>
       <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
+      <c r="G27" s="10" t="s">
+        <v>58</v>
+      </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
@@ -1866,17 +1892,19 @@
         <v>9</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E28" s="2" t="n">
         <f aca="false">A27</f>
         <v>26</v>
       </c>
       <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
+      <c r="G28" s="10" t="s">
+        <v>61</v>
+      </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
@@ -1905,10 +1933,10 @@
         <v>9</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E29" s="2" t="n">
         <f aca="false">A27</f>
@@ -1944,10 +1972,10 @@
         <v>9</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E30" s="2" t="n">
         <f aca="false">A27</f>
@@ -1983,10 +2011,10 @@
         <v>9</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E31" s="2" t="n">
         <f aca="false">A2</f>
@@ -2022,10 +2050,10 @@
         <v>9</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E32" s="2" t="n">
         <f aca="false">A31</f>
@@ -2061,10 +2089,10 @@
         <v>9</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E33" s="2" t="n">
         <f aca="false">A32</f>
@@ -2100,10 +2128,10 @@
         <v>9</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E34" s="2" t="n">
         <f aca="false">A32</f>
@@ -2139,17 +2167,19 @@
         <v>9</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E35" s="2" t="n">
         <f aca="false">A32</f>
         <v>31</v>
       </c>
       <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
+      <c r="G35" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
@@ -2178,10 +2208,10 @@
         <v>9</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E36" s="2" t="n">
         <f aca="false">A31</f>
@@ -2217,10 +2247,10 @@
         <v>9</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E37" s="2" t="n">
         <f aca="false">A36</f>
@@ -2256,10 +2286,10 @@
         <v>9</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="E38" s="2" t="n">
         <f aca="false">A37</f>
@@ -2332,10 +2362,10 @@
         <v>9</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="E40" s="2" t="n">
         <f aca="false">A39</f>
@@ -2371,10 +2401,10 @@
         <v>9</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E41" s="2" t="n">
         <f aca="false">A39</f>
@@ -2410,10 +2440,10 @@
         <v>9</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="E42" s="2" t="n">
         <f aca="false">A39</f>
@@ -2449,10 +2479,10 @@
         <v>9</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E43" s="2" t="n">
         <f aca="false">A39</f>
@@ -2488,14 +2518,14 @@
         <v>9</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
@@ -2526,10 +2556,10 @@
         <v>9</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="E45" s="2" t="n">
         <f aca="false">A44</f>
@@ -2565,10 +2595,10 @@
         <v>9</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="E46" s="2" t="n">
         <f aca="false">A45</f>
@@ -2604,10 +2634,10 @@
         <v>9</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="E47" s="2" t="n">
         <f aca="false">A46</f>
@@ -2643,10 +2673,10 @@
         <v>9</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="E48" s="2" t="n">
         <f aca="false">A46</f>
@@ -2682,10 +2712,10 @@
         <v>9</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="E49" s="2" t="n">
         <f aca="false">A46</f>
@@ -2721,10 +2751,10 @@
         <v>9</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="E50" s="2" t="n">
         <f aca="false">A46</f>
@@ -2760,10 +2790,10 @@
         <v>9</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="E51" s="2" t="n">
         <f aca="false">A46</f>
@@ -2799,10 +2829,10 @@
         <v>9</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="E52" s="2" t="n">
         <f aca="false">A45</f>
@@ -2831,19 +2861,19 @@
       <c r="Z52" s="2"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="10" t="n">
+      <c r="A53" s="11" t="n">
         <v>52</v>
       </c>
-      <c r="B53" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C53" s="10" t="s">
+      <c r="B53" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C53" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D53" s="10" t="s">
+      <c r="D53" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E53" s="10"/>
+      <c r="E53" s="11"/>
       <c r="F53" s="2" t="s">
         <v>12</v>
       </c>
@@ -2868,19 +2898,19 @@
       <c r="Z53" s="2"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="10" t="n">
+      <c r="A54" s="11" t="n">
         <v>53</v>
       </c>
-      <c r="B54" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C54" s="10" t="s">
+      <c r="B54" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C54" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D54" s="10" t="s">
+      <c r="D54" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E54" s="10" t="n">
+      <c r="E54" s="11" t="n">
         <f aca="false">A53</f>
         <v>52</v>
       </c>
@@ -2906,17 +2936,17 @@
       <c r="Z54" s="2"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="10" t="n">
+      <c r="A55" s="11" t="n">
         <v>54</v>
       </c>
-      <c r="B55" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C55" s="10" t="s">
+      <c r="B55" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C55" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D55" s="10"/>
-      <c r="E55" s="10" t="n">
+      <c r="D55" s="11"/>
+      <c r="E55" s="11" t="n">
         <f aca="false">A54</f>
         <v>53</v>
       </c>
@@ -2942,19 +2972,19 @@
       <c r="Z55" s="2"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="10" t="n">
+      <c r="A56" s="11" t="n">
         <v>55</v>
       </c>
-      <c r="B56" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C56" s="10" t="s">
+      <c r="B56" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C56" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D56" s="10" t="s">
+      <c r="D56" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E56" s="10" t="n">
+      <c r="E56" s="11" t="n">
         <f aca="false">A55</f>
         <v>54</v>
       </c>
@@ -2980,19 +3010,19 @@
       <c r="Z56" s="2"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="10" t="n">
+      <c r="A57" s="11" t="n">
         <v>56</v>
       </c>
-      <c r="B57" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C57" s="10" t="s">
+      <c r="B57" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C57" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D57" s="10" t="s">
+      <c r="D57" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E57" s="10" t="n">
+      <c r="E57" s="11" t="n">
         <f aca="false">A55</f>
         <v>54</v>
       </c>
@@ -3018,19 +3048,19 @@
       <c r="Z57" s="2"/>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="10" t="n">
+      <c r="A58" s="11" t="n">
         <v>57</v>
       </c>
-      <c r="B58" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C58" s="10" t="s">
+      <c r="B58" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C58" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D58" s="10" t="s">
+      <c r="D58" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E58" s="10" t="n">
+      <c r="E58" s="11" t="n">
         <f aca="false">A55</f>
         <v>54</v>
       </c>
@@ -3056,17 +3086,17 @@
       <c r="Z58" s="2"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="10" t="n">
+      <c r="A59" s="11" t="n">
         <v>58</v>
       </c>
-      <c r="B59" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C59" s="10" t="s">
+      <c r="B59" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C59" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D59" s="10"/>
-      <c r="E59" s="10" t="n">
+      <c r="D59" s="11"/>
+      <c r="E59" s="11" t="n">
         <f aca="false">A55</f>
         <v>54</v>
       </c>
@@ -3092,19 +3122,19 @@
       <c r="Z59" s="2"/>
     </row>
     <row r="60" customFormat="false" ht="173.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="10" t="n">
+      <c r="A60" s="11" t="n">
         <v>59</v>
       </c>
-      <c r="B60" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C60" s="10" t="s">
+      <c r="B60" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C60" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D60" s="11" t="s">
+      <c r="D60" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E60" s="10" t="n">
+      <c r="E60" s="11" t="n">
         <f aca="false">A59</f>
         <v>58</v>
       </c>
@@ -3130,19 +3160,19 @@
       <c r="Z60" s="2"/>
     </row>
     <row r="61" customFormat="false" ht="276.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="10" t="n">
+      <c r="A61" s="11" t="n">
         <v>60</v>
       </c>
-      <c r="B61" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C61" s="12" t="s">
+      <c r="B61" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C61" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D61" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="E61" s="10" t="n">
+      <c r="D61" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="E61" s="11" t="n">
         <f aca="false">A59</f>
         <v>58</v>
       </c>
@@ -3168,19 +3198,19 @@
       <c r="Z61" s="2"/>
     </row>
     <row r="62" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="10" t="n">
+      <c r="A62" s="11" t="n">
         <v>61</v>
       </c>
-      <c r="B62" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C62" s="12" t="s">
+      <c r="B62" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C62" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D62" s="13" t="s">
+      <c r="D62" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="E62" s="10" t="n">
+      <c r="E62" s="11" t="n">
         <f aca="false">A59</f>
         <v>58</v>
       </c>
@@ -3206,19 +3236,19 @@
       <c r="Z62" s="2"/>
     </row>
     <row r="63" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="10" t="n">
+      <c r="A63" s="11" t="n">
         <v>62</v>
       </c>
-      <c r="B63" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C63" s="10" t="s">
+      <c r="B63" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C63" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D63" s="11" t="s">
+      <c r="D63" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E63" s="10" t="n">
+      <c r="E63" s="11" t="n">
         <f aca="false">A53</f>
         <v>52</v>
       </c>
@@ -3244,17 +3274,17 @@
       <c r="Z63" s="2"/>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="10" t="n">
+      <c r="A64" s="11" t="n">
         <v>63</v>
       </c>
-      <c r="B64" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C64" s="10" t="s">
+      <c r="B64" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C64" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D64" s="10"/>
-      <c r="E64" s="10" t="n">
+      <c r="D64" s="11"/>
+      <c r="E64" s="11" t="n">
         <f aca="false">A63</f>
         <v>62</v>
       </c>
@@ -3280,17 +3310,17 @@
       <c r="Z64" s="2"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="10" t="n">
+      <c r="A65" s="11" t="n">
         <v>64</v>
       </c>
-      <c r="B65" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C65" s="10" t="s">
+      <c r="B65" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C65" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D65" s="10"/>
-      <c r="E65" s="10" t="n">
+      <c r="D65" s="11"/>
+      <c r="E65" s="11" t="n">
         <f aca="false">A64</f>
         <v>63</v>
       </c>
@@ -3316,17 +3346,17 @@
       <c r="Z65" s="2"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="10" t="n">
+      <c r="A66" s="11" t="n">
         <v>65</v>
       </c>
-      <c r="B66" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C66" s="10" t="s">
+      <c r="B66" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C66" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D66" s="10"/>
-      <c r="E66" s="10" t="n">
+      <c r="D66" s="11"/>
+      <c r="E66" s="11" t="n">
         <f aca="false">A65</f>
         <v>64</v>
       </c>
@@ -3352,19 +3382,19 @@
       <c r="Z66" s="2"/>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="10" t="n">
+      <c r="A67" s="11" t="n">
         <v>66</v>
       </c>
-      <c r="B67" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C67" s="10" t="s">
+      <c r="B67" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C67" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D67" s="14" t="s">
+      <c r="D67" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="E67" s="10" t="n">
+      <c r="E67" s="11" t="n">
         <f aca="false">A66</f>
         <v>65</v>
       </c>
@@ -3390,19 +3420,19 @@
       <c r="Z67" s="2"/>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="10" t="n">
+      <c r="A68" s="11" t="n">
         <v>67</v>
       </c>
-      <c r="B68" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C68" s="14" t="s">
+      <c r="B68" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C68" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="D68" s="10" t="s">
+      <c r="D68" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="E68" s="10" t="n">
+      <c r="E68" s="11" t="n">
         <f aca="false">A66</f>
         <v>65</v>
       </c>
@@ -3428,17 +3458,17 @@
       <c r="Z68" s="2"/>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="10" t="n">
+      <c r="A69" s="11" t="n">
         <v>68</v>
       </c>
-      <c r="B69" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C69" s="10" t="s">
+      <c r="B69" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C69" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D69" s="10"/>
-      <c r="E69" s="10" t="n">
+      <c r="D69" s="11"/>
+      <c r="E69" s="11" t="n">
         <f aca="false">A65</f>
         <v>64</v>
       </c>
@@ -3464,19 +3494,19 @@
       <c r="Z69" s="2"/>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="10" t="n">
+      <c r="A70" s="11" t="n">
         <v>69</v>
       </c>
-      <c r="B70" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C70" s="10" t="s">
+      <c r="B70" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C70" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="D70" s="10" t="s">
+      <c r="D70" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="E70" s="10" t="n">
+      <c r="E70" s="11" t="n">
         <f aca="false">A69</f>
         <v>68</v>
       </c>
@@ -3502,19 +3532,19 @@
       <c r="Z70" s="2"/>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="10" t="n">
+      <c r="A71" s="11" t="n">
         <v>70</v>
       </c>
-      <c r="B71" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C71" s="10" t="s">
+      <c r="B71" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C71" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="D71" s="10" t="s">
+      <c r="D71" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E71" s="10" t="n">
+      <c r="E71" s="11" t="n">
         <f aca="false">A65</f>
         <v>64</v>
       </c>
@@ -3540,17 +3570,17 @@
       <c r="Z71" s="2"/>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="10" t="n">
+      <c r="A72" s="11" t="n">
         <v>71</v>
       </c>
-      <c r="B72" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C72" s="10" t="s">
+      <c r="B72" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C72" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="D72" s="10"/>
-      <c r="E72" s="10" t="n">
+      <c r="D72" s="11"/>
+      <c r="E72" s="11" t="n">
         <f aca="false">A64</f>
         <v>63</v>
       </c>
@@ -3576,17 +3606,17 @@
       <c r="Z72" s="2"/>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="10" t="n">
+      <c r="A73" s="11" t="n">
         <v>72</v>
       </c>
-      <c r="B73" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C73" s="10" t="s">
+      <c r="B73" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C73" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="D73" s="10"/>
-      <c r="E73" s="10" t="n">
+      <c r="D73" s="11"/>
+      <c r="E73" s="11" t="n">
         <f aca="false">A72</f>
         <v>71</v>
       </c>
@@ -3612,19 +3642,19 @@
       <c r="Z73" s="2"/>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="10" t="n">
+      <c r="A74" s="11" t="n">
         <v>73</v>
       </c>
-      <c r="B74" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C74" s="10" t="s">
+      <c r="B74" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C74" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D74" s="10" t="s">
+      <c r="D74" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="E74" s="10" t="n">
+      <c r="E74" s="11" t="n">
         <f aca="false">A73</f>
         <v>72</v>
       </c>
@@ -3650,19 +3680,19 @@
       <c r="Z74" s="2"/>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="10" t="n">
+      <c r="A75" s="11" t="n">
         <v>74</v>
       </c>
-      <c r="B75" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C75" s="14" t="s">
+      <c r="B75" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C75" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="D75" s="10" t="s">
+      <c r="D75" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E75" s="10" t="n">
+      <c r="E75" s="11" t="n">
         <f aca="false">A73</f>
         <v>72</v>
       </c>
@@ -3688,19 +3718,19 @@
       <c r="Z75" s="2"/>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="10" t="n">
+      <c r="A76" s="11" t="n">
         <v>75</v>
       </c>
-      <c r="B76" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C76" s="10" t="s">
+      <c r="B76" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C76" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D76" s="10" t="s">
+      <c r="D76" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="E76" s="10" t="n">
+      <c r="E76" s="11" t="n">
         <f aca="false">A72</f>
         <v>71</v>
       </c>
@@ -3726,19 +3756,19 @@
       <c r="Z76" s="2"/>
     </row>
     <row r="77" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="10" t="n">
+      <c r="A77" s="11" t="n">
         <v>76</v>
       </c>
-      <c r="B77" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C77" s="10" t="s">
+      <c r="B77" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C77" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="D77" s="11" t="s">
+      <c r="D77" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="E77" s="10" t="n">
+      <c r="E77" s="11" t="n">
         <f aca="false">A53</f>
         <v>52</v>
       </c>
@@ -3764,17 +3794,17 @@
       <c r="Z77" s="2"/>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="10" t="n">
+      <c r="A78" s="11" t="n">
         <v>77</v>
       </c>
-      <c r="B78" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C78" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="D78" s="10"/>
-      <c r="E78" s="10" t="n">
+      <c r="B78" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C78" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D78" s="11"/>
+      <c r="E78" s="11" t="n">
         <f aca="false">A77</f>
         <v>76</v>
       </c>
@@ -3800,19 +3830,19 @@
       <c r="Z78" s="2"/>
     </row>
     <row r="79" customFormat="false" ht="173.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="10" t="n">
+      <c r="A79" s="11" t="n">
         <v>78</v>
       </c>
-      <c r="B79" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C79" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D79" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="E79" s="10" t="n">
+      <c r="B79" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C79" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D79" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E79" s="11" t="n">
         <f aca="false">A78</f>
         <v>77</v>
       </c>
@@ -3838,19 +3868,19 @@
       <c r="Z79" s="2"/>
     </row>
     <row r="80" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="10" t="n">
+      <c r="A80" s="11" t="n">
         <v>79</v>
       </c>
-      <c r="B80" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C80" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="D80" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E80" s="10" t="n">
+      <c r="B80" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C80" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D80" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E80" s="11" t="n">
         <f aca="false">A78</f>
         <v>77</v>
       </c>
@@ -3876,19 +3906,19 @@
       <c r="Z80" s="2"/>
     </row>
     <row r="81" customFormat="false" ht="127.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="10" t="n">
+      <c r="A81" s="11" t="n">
         <v>80</v>
       </c>
-      <c r="B81" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C81" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="D81" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="E81" s="10" t="n">
+      <c r="B81" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C81" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D81" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E81" s="11" t="n">
         <f aca="false">A78</f>
         <v>77</v>
       </c>
@@ -3914,19 +3944,19 @@
       <c r="Z81" s="2"/>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="10" t="n">
+      <c r="A82" s="11" t="n">
         <v>81</v>
       </c>
-      <c r="B82" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C82" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="D82" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="E82" s="10" t="n">
+      <c r="B82" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C82" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D82" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E82" s="11" t="n">
         <f aca="false">A53</f>
         <v>52</v>
       </c>
@@ -3952,19 +3982,19 @@
       <c r="Z82" s="2"/>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="10" t="n">
+      <c r="A83" s="11" t="n">
         <v>82</v>
       </c>
-      <c r="B83" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C83" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D83" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="E83" s="10" t="n">
+      <c r="B83" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C83" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="D83" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E83" s="11" t="n">
         <f aca="false">A82</f>
         <v>81</v>
       </c>
@@ -3990,19 +4020,19 @@
       <c r="Z83" s="2"/>
     </row>
     <row r="84" customFormat="false" ht="92.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="10" t="n">
+      <c r="A84" s="11" t="n">
         <v>83</v>
       </c>
-      <c r="B84" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C84" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D84" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="E84" s="10" t="n">
+      <c r="B84" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C84" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="D84" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="E84" s="11" t="n">
         <f aca="false">A83</f>
         <v>82</v>
       </c>
@@ -4028,19 +4058,19 @@
       <c r="Z84" s="2"/>
     </row>
     <row r="85" customFormat="false" ht="81.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="10" t="n">
+      <c r="A85" s="11" t="n">
         <v>84</v>
       </c>
-      <c r="B85" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C85" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="D85" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="E85" s="10" t="n">
+      <c r="B85" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C85" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D85" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E85" s="11" t="n">
         <f aca="false">A83</f>
         <v>82</v>
       </c>
@@ -4066,19 +4096,19 @@
       <c r="Z85" s="2"/>
     </row>
     <row r="86" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="10" t="n">
+      <c r="A86" s="11" t="n">
         <v>85</v>
       </c>
-      <c r="B86" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C86" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="D86" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="E86" s="10" t="n">
+      <c r="B86" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C86" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D86" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E86" s="11" t="n">
         <f aca="false">A83</f>
         <v>82</v>
       </c>
@@ -4104,19 +4134,19 @@
       <c r="Z86" s="2"/>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="10" t="n">
+      <c r="A87" s="11" t="n">
         <v>86</v>
       </c>
-      <c r="B87" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C87" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="D87" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="E87" s="10" t="n">
+      <c r="B87" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C87" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D87" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="E87" s="11" t="n">
         <f aca="false">A82</f>
         <v>81</v>
       </c>
@@ -4142,19 +4172,19 @@
       <c r="Z87" s="2"/>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="10" t="n">
+      <c r="A88" s="11" t="n">
         <v>87</v>
       </c>
-      <c r="B88" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C88" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="D88" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="E88" s="10" t="n">
+      <c r="B88" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C88" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D88" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="E88" s="11" t="n">
         <f aca="false">A87</f>
         <v>86</v>
       </c>
@@ -4180,19 +4210,19 @@
       <c r="Z88" s="2"/>
     </row>
     <row r="89" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="10" t="n">
+      <c r="A89" s="11" t="n">
         <v>88</v>
       </c>
-      <c r="B89" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C89" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D89" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="E89" s="10" t="n">
+      <c r="B89" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C89" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D89" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="E89" s="11" t="n">
         <f aca="false">A88</f>
         <v>87</v>
       </c>
@@ -4218,17 +4248,17 @@
       <c r="Z89" s="2"/>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="10" t="n">
+      <c r="A90" s="11" t="n">
         <v>89</v>
       </c>
-      <c r="B90" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C90" s="10" t="s">
+      <c r="B90" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C90" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D90" s="10"/>
-      <c r="E90" s="10" t="n">
+      <c r="D90" s="11"/>
+      <c r="E90" s="11" t="n">
         <f aca="false">A82</f>
         <v>81</v>
       </c>
@@ -4254,19 +4284,19 @@
       <c r="Z90" s="2"/>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="10" t="n">
+      <c r="A91" s="11" t="n">
         <v>90</v>
       </c>
-      <c r="B91" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C91" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="D91" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="E91" s="10" t="n">
+      <c r="B91" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C91" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D91" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="E91" s="11" t="n">
         <f aca="false">A90</f>
         <v>89</v>
       </c>
@@ -4292,19 +4322,19 @@
       <c r="Z91" s="2"/>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="10" t="n">
+      <c r="A92" s="11" t="n">
         <v>91</v>
       </c>
-      <c r="B92" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C92" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="D92" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="E92" s="10" t="n">
+      <c r="B92" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C92" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D92" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="E92" s="11" t="n">
         <f aca="false">A90</f>
         <v>89</v>
       </c>
@@ -4330,19 +4360,19 @@
       <c r="Z92" s="2"/>
     </row>
     <row r="93" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="10" t="n">
+      <c r="A93" s="11" t="n">
         <v>92</v>
       </c>
-      <c r="B93" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C93" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="D93" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="E93" s="10" t="n">
+      <c r="B93" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C93" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D93" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="E93" s="11" t="n">
         <f aca="false">A90</f>
         <v>89</v>
       </c>
@@ -4368,19 +4398,19 @@
       <c r="Z93" s="2"/>
     </row>
     <row r="94" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="10" t="n">
+      <c r="A94" s="11" t="n">
         <v>93</v>
       </c>
-      <c r="B94" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C94" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="D94" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="E94" s="10" t="n">
+      <c r="B94" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C94" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D94" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="E94" s="11" t="n">
         <f aca="false">A90</f>
         <v>89</v>
       </c>
@@ -4406,21 +4436,21 @@
       <c r="Z94" s="2"/>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="10" t="n">
+      <c r="A95" s="11" t="n">
         <v>94</v>
       </c>
-      <c r="B95" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C95" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="D95" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="E95" s="10"/>
+      <c r="B95" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C95" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="D95" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E95" s="11"/>
       <c r="F95" s="2" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="H95" s="2"/>
       <c r="I95" s="2"/>
@@ -4443,19 +4473,19 @@
       <c r="Z95" s="2"/>
     </row>
     <row r="96" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="10" t="n">
+      <c r="A96" s="11" t="n">
         <v>95</v>
       </c>
-      <c r="B96" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C96" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D96" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="E96" s="10" t="n">
+      <c r="B96" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C96" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="D96" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="E96" s="11" t="n">
         <f aca="false">A95</f>
         <v>94</v>
       </c>
@@ -4481,19 +4511,19 @@
       <c r="Z96" s="2"/>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="10" t="n">
+      <c r="A97" s="11" t="n">
         <v>96</v>
       </c>
-      <c r="B97" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C97" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="D97" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="E97" s="10" t="n">
+      <c r="B97" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C97" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="D97" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="E97" s="11" t="n">
         <f aca="false">A96</f>
         <v>95</v>
       </c>
@@ -4519,19 +4549,19 @@
       <c r="Z97" s="2"/>
     </row>
     <row r="98" customFormat="false" ht="115.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="10" t="n">
+      <c r="A98" s="11" t="n">
         <v>97</v>
       </c>
-      <c r="B98" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C98" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="D98" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="E98" s="10" t="n">
+      <c r="B98" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C98" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="D98" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="E98" s="11" t="n">
         <f aca="false">A97</f>
         <v>96</v>
       </c>
@@ -4557,19 +4587,19 @@
       <c r="Z98" s="2"/>
     </row>
     <row r="99" customFormat="false" ht="69.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="10" t="n">
+      <c r="A99" s="11" t="n">
         <v>98</v>
       </c>
-      <c r="B99" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C99" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="D99" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="E99" s="10" t="n">
+      <c r="B99" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C99" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D99" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="E99" s="11" t="n">
         <f aca="false">A97</f>
         <v>96</v>
       </c>
@@ -4596,19 +4626,19 @@
       <c r="Z99" s="2"/>
     </row>
     <row r="100" customFormat="false" ht="35.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="10" t="n">
+      <c r="A100" s="11" t="n">
         <v>99</v>
       </c>
-      <c r="B100" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C100" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="D100" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="E100" s="10" t="n">
+      <c r="B100" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C100" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D100" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E100" s="11" t="n">
         <f aca="false">A97</f>
         <v>96</v>
       </c>
@@ -4635,19 +4665,19 @@
       <c r="Z100" s="2"/>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="10" t="n">
+      <c r="A101" s="11" t="n">
         <v>100</v>
       </c>
-      <c r="B101" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C101" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="D101" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="E101" s="10" t="n">
+      <c r="B101" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C101" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D101" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E101" s="11" t="n">
         <f aca="false">A97</f>
         <v>96</v>
       </c>
@@ -4674,19 +4704,19 @@
       <c r="Z101" s="2"/>
     </row>
     <row r="102" customFormat="false" ht="58.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="10" t="n">
+      <c r="A102" s="11" t="n">
         <v>101</v>
       </c>
-      <c r="B102" s="10" t="s">
+      <c r="B102" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C102" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="C102" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="D102" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="E102" s="10" t="n">
+      <c r="D102" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="E102" s="11" t="n">
         <f aca="false">A97</f>
         <v>96</v>
       </c>
@@ -4713,19 +4743,19 @@
       <c r="Z102" s="2"/>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="10" t="n">
+      <c r="A103" s="11" t="n">
         <v>102</v>
       </c>
-      <c r="B103" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C103" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="D103" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="E103" s="10" t="n">
+      <c r="B103" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C103" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="D103" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="E103" s="11" t="n">
         <f aca="false">A96</f>
         <v>95</v>
       </c>

</xml_diff>